<commit_message>
R&R 1st round done
finished the 1st round R&R; added PCA analysis to do model selection; completed documentations; published to GitHub
</commit_message>
<xml_diff>
--- a/data/CHARLS_CITY.xlsx
+++ b/data/CHARLS_CITY.xlsx
@@ -782,7 +782,7 @@
         <v>19168.7209302326</v>
       </c>
       <c r="AK2" s="0">
-        <v>11193.7735849057</v>
+        <v>1.11937735849057</v>
       </c>
       <c r="AL2" s="0">
         <v>3632.29508196721</v>
@@ -977,7 +977,7 @@
         <v>17787.8787878788</v>
       </c>
       <c r="AK3" s="0">
-        <v>10388.9108910891</v>
+        <v>1.03889108910891</v>
       </c>
       <c r="AL3" s="0">
         <v>9528.52941176471</v>
@@ -1172,7 +1172,7 @@
         <v>29107.746835443</v>
       </c>
       <c r="AK4" s="0">
-        <v>16144.8073394495</v>
+        <v>1.61448073394495</v>
       </c>
       <c r="AL4" s="0">
         <v>5797.12</v>
@@ -1367,7 +1367,7 @@
         <v>13450.0757575758</v>
       </c>
       <c r="AK5" s="0">
-        <v>9348.13793103448</v>
+        <v>0.934813793103448</v>
       </c>
       <c r="AL5" s="0">
         <v>1897.61904761905</v>
@@ -1562,7 +1562,7 @@
         <v>14370.0069204152</v>
       </c>
       <c r="AK6" s="0">
-        <v>7988.28387096774</v>
+        <v>0.798828387096774</v>
       </c>
       <c r="AL6" s="0">
         <v>5159.24347826087</v>
@@ -1757,7 +1757,7 @@
         <v>26686.0108471074</v>
       </c>
       <c r="AK7" s="0">
-        <v>15295.2709363759</v>
+        <v>1.52952709363759</v>
       </c>
       <c r="AL7" s="0">
         <v>4808.72093023256</v>
@@ -1952,7 +1952,7 @@
         <v>56573.5033557047</v>
       </c>
       <c r="AK8" s="0">
-        <v>32785.0259067358</v>
+        <v>3.27850259067358</v>
       </c>
       <c r="AL8" s="0">
         <v>225.478260869565</v>
@@ -2147,7 +2147,7 @@
         <v>89576.4556962025</v>
       </c>
       <c r="AK9" s="0">
-        <v>45726.4516129032</v>
+        <v>4.57264516129032</v>
       </c>
       <c r="AL9" s="0">
         <v>1900</v>
@@ -2342,7 +2342,7 @@
         <v>34761.1267605634</v>
       </c>
       <c r="AK10" s="0">
-        <v>23030.099009901</v>
+        <v>2.3030099009901</v>
       </c>
       <c r="AL10" s="0">
         <v>1762.5</v>
@@ -2537,7 +2537,7 @@
         <v>19551.8076923077</v>
       </c>
       <c r="AK11" s="0">
-        <v>10931.7931034483</v>
+        <v>1.09317931034483</v>
       </c>
       <c r="AL11" s="0">
         <v>3368.9247311828</v>
@@ -2732,7 +2732,7 @@
         <v>40479.3191489362</v>
       </c>
       <c r="AK12" s="0">
-        <v>23638.0281690141</v>
+        <v>2.36380281690141</v>
       </c>
       <c r="AL12" s="0">
         <v>3852.38095238095</v>
@@ -2927,7 +2927,7 @@
         <v>40230.3636363636</v>
       </c>
       <c r="AK13" s="0">
-        <v>23148.8253968254</v>
+        <v>2.31488253968254</v>
       </c>
       <c r="AL13" s="0">
         <v>9914.17721518987</v>
@@ -3122,7 +3122,7 @@
         <v>36612.0869565217</v>
       </c>
       <c r="AK14" s="0">
-        <v>21344.4761904762</v>
+        <v>2.13444761904762</v>
       </c>
       <c r="AL14" s="0">
         <v>25728.8</v>
@@ -3317,7 +3317,7 @@
         <v>14268.1460674157</v>
       </c>
       <c r="AK15" s="0">
-        <v>5459.96666666667</v>
+        <v>0.545996666666667</v>
       </c>
       <c r="AL15" s="0">
         <v>5917.02127659574</v>
@@ -3512,7 +3512,7 @@
         <v>30623.075</v>
       </c>
       <c r="AK16" s="0">
-        <v>23116.3333333333</v>
+        <v>2.31163333333333</v>
       </c>
       <c r="AL16" s="0">
         <v>5163.26530612245</v>
@@ -3707,7 +3707,7 @@
         <v>14612.1296296296</v>
       </c>
       <c r="AK17" s="0">
-        <v>5827.71929824561</v>
+        <v>0.582771929824562</v>
       </c>
       <c r="AL17" s="0">
         <v>1904.61538461538</v>
@@ -3902,7 +3902,7 @@
         <v>26917.8333440061</v>
       </c>
       <c r="AK18" s="0">
-        <v>14173.9780597928</v>
+        <v>1.41739780597928</v>
       </c>
       <c r="AL18" s="0">
         <v>3019.05737704918</v>
@@ -4097,7 +4097,7 @@
         <v>18825.9461538462</v>
       </c>
       <c r="AK19" s="0">
-        <v>13227.0652173913</v>
+        <v>1.32270652173913</v>
       </c>
       <c r="AL19" s="0">
         <v>2920.96774193548</v>
@@ -4292,7 +4292,7 @@
         <v>37388.2894736842</v>
       </c>
       <c r="AK20" s="0">
-        <v>21465.6456692913</v>
+        <v>2.14656456692913</v>
       </c>
       <c r="AL20" s="0">
         <v>4459.13978494624</v>
@@ -4487,7 +4487,7 @@
         <v>18602.7024793388</v>
       </c>
       <c r="AK21" s="0">
-        <v>6799.38970588235</v>
+        <v>0.679938970588235</v>
       </c>
       <c r="AL21" s="0">
         <v>3538.94859813084</v>
@@ -4682,7 +4682,7 @@
         <v>34887.2203389831</v>
       </c>
       <c r="AK22" s="0">
-        <v>20844.301369863</v>
+        <v>2.0844301369863</v>
       </c>
       <c r="AL22" s="0">
         <v>4830.94339622641</v>
@@ -4877,7 +4877,7 @@
         <v>27056.3846153846</v>
       </c>
       <c r="AK23" s="0">
-        <v>14470.1481481481</v>
+        <v>1.44701481481481</v>
       </c>
       <c r="AL23" s="0">
         <v>8615.74468085106</v>
@@ -5072,7 +5072,7 @@
         <v>15199.1684210526</v>
       </c>
       <c r="AK24" s="0">
-        <v>7274.77678571429</v>
+        <v>0.727477678571429</v>
       </c>
       <c r="AL24" s="0">
         <v>8034.8051948052</v>
@@ -5267,7 +5267,7 @@
         <v>25964.9142857143</v>
       </c>
       <c r="AK25" s="0">
-        <v>17150.7155172414</v>
+        <v>1.71507155172414</v>
       </c>
       <c r="AL25" s="0">
         <v>2753.64705882353</v>
@@ -5462,7 +5462,7 @@
         <v>44658.9946157095</v>
       </c>
       <c r="AK26" s="0">
-        <v>26813.3219047546</v>
+        <v>2.68133219047546</v>
       </c>
       <c r="AL26" s="0">
         <v>18582.8571428571</v>
@@ -5657,7 +5657,7 @@
         <v>35555.4583333333</v>
       </c>
       <c r="AK27" s="0">
-        <v>23482.347826087</v>
+        <v>2.3482347826087</v>
       </c>
       <c r="AL27" s="0">
         <v>399.915492957746</v>
@@ -5852,7 +5852,7 @@
         <v>51318.9607843137</v>
       </c>
       <c r="AK28" s="0">
-        <v>34252.534351145</v>
+        <v>3.4252534351145</v>
       </c>
       <c r="AL28" s="0">
         <v>11581.5825242718</v>
@@ -6047,7 +6047,7 @@
         <v>8954.11320754717</v>
       </c>
       <c r="AK29" s="0">
-        <v>5991.67741935484</v>
+        <v>0.599167741935484</v>
       </c>
       <c r="AL29" s="0">
         <v>4687.7358490566</v>
@@ -6242,7 +6242,7 @@
         <v>27738.0223473837</v>
       </c>
       <c r="AK30" s="0">
-        <v>15522.2391696506</v>
+        <v>1.55222391696506</v>
       </c>
       <c r="AL30" s="0">
         <v>4190</v>
@@ -6437,7 +6437,7 @@
         <v>12727.8333333333</v>
       </c>
       <c r="AK31" s="0">
-        <v>8283.86290322581</v>
+        <v>0.828386290322581</v>
       </c>
       <c r="AL31" s="0">
         <v>2010</v>
@@ -6632,7 +6632,7 @@
         <v>35601.9496402878</v>
       </c>
       <c r="AK32" s="0">
-        <v>20167.0890052356</v>
+        <v>2.01670890052356</v>
       </c>
       <c r="AL32" s="0">
         <v>1398.59649122807</v>
@@ -6827,7 +6827,7 @@
         <v>51211.6001059322</v>
       </c>
       <c r="AK33" s="0">
-        <v>27851.9123507725</v>
+        <v>2.78519123507725</v>
       </c>
       <c r="AL33" s="0">
         <v>4004.34782608696</v>
@@ -7022,7 +7022,7 @@
         <v>64655.5714285714</v>
       </c>
       <c r="AK34" s="0">
-        <v>36455.0882352941</v>
+        <v>3.64550882352941</v>
       </c>
       <c r="AL34" s="0">
         <v>2500</v>
@@ -7217,7 +7217,7 @@
         <v>41442.9655172414</v>
       </c>
       <c r="AK35" s="0">
-        <v>26073.5588235294</v>
+        <v>2.60735588235294</v>
       </c>
       <c r="AL35" s="0">
         <v>3125</v>
@@ -7412,7 +7412,7 @@
         <v>16072.3513513514</v>
       </c>
       <c r="AK36" s="0">
-        <v>8359.44444444445</v>
+        <v>0.835944444444444</v>
       </c>
       <c r="AL36" s="0">
         <v>6239.39316239316</v>
@@ -7607,7 +7607,7 @@
         <v>22705.4453125</v>
       </c>
       <c r="AK37" s="0">
-        <v>13210.9236696478</v>
+        <v>1.32109236696478</v>
       </c>
       <c r="AL37" s="0">
         <v>2855.39682539683</v>
@@ -7802,7 +7802,7 @@
         <v>63787.3684210526</v>
       </c>
       <c r="AK38" s="0">
-        <v>57904.1025641026</v>
+        <v>5.79041025641026</v>
       </c>
       <c r="AL38" s="0">
         <v>6564.10256410256</v>
@@ -7997,7 +7997,7 @@
         <v>35597.641509434</v>
       </c>
       <c r="AK39" s="0">
-        <v>25865.203125</v>
+        <v>2.5865203125</v>
       </c>
       <c r="AL39" s="0">
         <v>3234.63414634146</v>
@@ -8192,7 +8192,7 @@
         <v>16707.025</v>
       </c>
       <c r="AK40" s="0">
-        <v>37189.2736842105</v>
+        <v>3.71892736842105</v>
       </c>
       <c r="AL40" s="0">
         <v>13594.4444444444</v>
@@ -8387,7 +8387,7 @@
         <v>22869.952681388</v>
       </c>
       <c r="AK41" s="0">
-        <v>10017.1615598886</v>
+        <v>1.00171615598886</v>
       </c>
       <c r="AL41" s="0">
         <v>9123.6015037594</v>
@@ -8582,7 +8582,7 @@
         <v>66283.537377451</v>
       </c>
       <c r="AK42" s="0">
-        <v>50253.0531546677</v>
+        <v>5.02530531546677</v>
       </c>
       <c r="AL42" s="0">
         <v>6995.12195121951</v>
@@ -8777,7 +8777,7 @@
         <v>38490.1758241758</v>
       </c>
       <c r="AK43" s="0">
-        <v>30718.1121495327</v>
+        <v>3.07181121495327</v>
       </c>
       <c r="AL43" s="0">
         <v>6956.34146341463</v>
@@ -8972,7 +8972,7 @@
         <v>29411.6029411765</v>
       </c>
       <c r="AK44" s="0">
-        <v>17992.1176470588</v>
+        <v>1.79921176470588</v>
       </c>
       <c r="AL44" s="0">
         <v>4267.96116504854</v>
@@ -9167,7 +9167,7 @@
         <v>15194.4358974359</v>
       </c>
       <c r="AK45" s="0">
-        <v>5833.64051968444</v>
+        <v>0.583364051968444</v>
       </c>
       <c r="AL45" s="0">
         <v>10403.1746031746</v>
@@ -9362,7 +9362,7 @@
         <v>39544.8972355769</v>
       </c>
       <c r="AK46" s="0">
-        <v>25448.4122971755</v>
+        <v>2.54484122971755</v>
       </c>
       <c r="AL46" s="0">
         <v>402.941176470588</v>
@@ -9557,7 +9557,7 @@
         <v>43859.4123894743</v>
       </c>
       <c r="AK47" s="0">
-        <v>24713.6336127387</v>
+        <v>2.47136336127387</v>
       </c>
       <c r="AL47" s="0">
         <v>2363.07692307692</v>
@@ -9752,7 +9752,7 @@
         <v>41749.9069475446</v>
       </c>
       <c r="AK48" s="0">
-        <v>23474.0516979836</v>
+        <v>2.34740516979836</v>
       </c>
       <c r="AL48" s="0">
         <v>8337.0101010101</v>
@@ -9947,7 +9947,7 @@
         <v>78204.0952380952</v>
       </c>
       <c r="AK49" s="0">
-        <v>42252.9545454545</v>
+        <v>4.22529545454545</v>
       </c>
       <c r="AL49" s="0">
         <v>31200</v>
@@ -10142,7 +10142,7 @@
         <v>69694.6</v>
       </c>
       <c r="AK50" s="0">
-        <v>37856.7924528302</v>
+        <v>3.78567924528302</v>
       </c>
       <c r="AL50" s="0">
         <v>17705.2631578947</v>
@@ -10337,7 +10337,7 @@
         <v>56338.4301423373</v>
       </c>
       <c r="AK51" s="0">
-        <v>25901.3599999322</v>
+        <v>2.59013599999322</v>
       </c>
       <c r="AL51" s="0">
         <v>-1406.66666666667</v>
@@ -10532,7 +10532,7 @@
         <v>19085.347826087</v>
       </c>
       <c r="AK52" s="0">
-        <v>12317.4383561644</v>
+        <v>1.23174383561644</v>
       </c>
       <c r="AL52" s="0">
         <v>3663.39285714286</v>
@@ -10727,7 +10727,7 @@
         <v>30545.2720588235</v>
       </c>
       <c r="AK53" s="0">
-        <v>15571.7198581154</v>
+        <v>1.55717198581154</v>
       </c>
       <c r="AL53" s="0">
         <v>3884.74747474747</v>
@@ -10922,7 +10922,7 @@
         <v>34260.8115942029</v>
       </c>
       <c r="AK54" s="0">
-        <v>20633.2083333333</v>
+        <v>2.06332083333333</v>
       </c>
       <c r="AL54" s="0">
         <v>9639.73684210526</v>
@@ -11117,7 +11117,7 @@
         <v>38652.5675675676</v>
       </c>
       <c r="AK55" s="0">
-        <v>24642.6206896552</v>
+        <v>2.46426206896552</v>
       </c>
       <c r="AL55" s="0">
         <v>4777.55102040816</v>
@@ -11312,7 +11312,7 @@
         <v>25066.0430107527</v>
       </c>
       <c r="AK56" s="0">
-        <v>15558.0186915888</v>
+        <v>1.55580186915888</v>
       </c>
       <c r="AL56" s="0">
         <v>16883.6111111111</v>
@@ -11507,7 +11507,7 @@
         <v>26956.8774193548</v>
       </c>
       <c r="AK57" s="0">
-        <v>16781.63507109</v>
+        <v>1.678163507109</v>
       </c>
       <c r="AL57" s="0">
         <v>4786.9696969697</v>
@@ -11702,7 +11702,7 @@
         <v>39387.4482758621</v>
       </c>
       <c r="AK58" s="0">
-        <v>24521.2173913043</v>
+        <v>2.45212173913043</v>
       </c>
       <c r="AL58" s="0">
         <v>0</v>
@@ -11897,7 +11897,7 @@
         <v>10686.8941176471</v>
       </c>
       <c r="AK59" s="0">
-        <v>5772.26923076923</v>
+        <v>0.577226923076923</v>
       </c>
       <c r="AL59" s="0">
         <v>3566.27450980392</v>
@@ -12092,7 +12092,7 @@
         <v>16896.6767676768</v>
       </c>
       <c r="AK60" s="0">
-        <v>11587.304</v>
+        <v>1.1587304</v>
       </c>
       <c r="AL60" s="0">
         <v>8845.98734177215</v>
@@ -12287,7 +12287,7 @@
         <v>33590.5688073394</v>
       </c>
       <c r="AK61" s="0">
-        <v>19006.6850393701</v>
+        <v>1.90066850393701</v>
       </c>
       <c r="AL61" s="0">
         <v>2152</v>
@@ -12482,7 +12482,7 @@
         <v>37680.8536585366</v>
       </c>
       <c r="AK62" s="0">
-        <v>17205.6790123457</v>
+        <v>1.72056790123457</v>
       </c>
       <c r="AL62" s="0">
         <v>8461.98412698413</v>
@@ -12677,7 +12677,7 @@
         <v>22647.3626373626</v>
       </c>
       <c r="AK63" s="0">
-        <v>14135.3978494624</v>
+        <v>1.41353978494624</v>
       </c>
       <c r="AL63" s="0">
         <v>1720.91503267974</v>
@@ -12872,7 +12872,7 @@
         <v>18225</v>
       </c>
       <c r="AK64" s="0">
-        <v>10523.5643564356</v>
+        <v>1.05235643564356</v>
       </c>
       <c r="AL64" s="0">
         <v>4645.85714285714</v>
@@ -13067,7 +13067,7 @@
         <v>19116.5891472868</v>
       </c>
       <c r="AK65" s="0">
-        <v>12700.8428571429</v>
+        <v>1.27008428571429</v>
       </c>
       <c r="AL65" s="0">
         <v>4668.28828828829</v>
@@ -13262,7 +13262,7 @@
         <v>27017.7079646018</v>
       </c>
       <c r="AK66" s="0">
-        <v>12938.1204379562</v>
+        <v>1.29381204379562</v>
       </c>
       <c r="AL66" s="0">
         <v>3166.88372093023</v>
@@ -13457,7 +13457,7 @@
         <v>13898.5454545455</v>
       </c>
       <c r="AK67" s="0">
-        <v>5765.92105263158</v>
+        <v>0.576592105263158</v>
       </c>
       <c r="AL67" s="0">
         <v>5851.64835164835</v>
@@ -13652,7 +13652,7 @@
         <v>34206.7288135593</v>
       </c>
       <c r="AK68" s="0">
-        <v>24794.8059701493</v>
+        <v>2.47948059701493</v>
       </c>
       <c r="AL68" s="0">
         <v>6764.36781609195</v>
@@ -13847,7 +13847,7 @@
         <v>72420.003503418</v>
       </c>
       <c r="AK69" s="0">
-        <v>34932.8702914044</v>
+        <v>3.49328702914044</v>
       </c>
       <c r="AL69" s="0">
         <v>2750.30769230769</v>
@@ -14042,7 +14042,7 @@
         <v>20752.7632653061</v>
       </c>
       <c r="AK70" s="0">
-        <v>14827.3756146098</v>
+        <v>1.48273756146098</v>
       </c>
       <c r="AL70" s="0">
         <v>5155.78010471204</v>
@@ -14237,7 +14237,7 @@
         <v>18455.9746835443</v>
       </c>
       <c r="AK71" s="0">
-        <v>10586.7741935484</v>
+        <v>1.05867741935484</v>
       </c>
       <c r="AL71" s="0">
         <v>5931.49473684211</v>
@@ -14432,7 +14432,7 @@
         <v>24460.2432432432</v>
       </c>
       <c r="AK72" s="0">
-        <v>8221.1214953271</v>
+        <v>0.82211214953271</v>
       </c>
       <c r="AL72" s="0">
         <v>6562.55</v>
@@ -14627,7 +14627,7 @@
         <v>35879.1847826087</v>
       </c>
       <c r="AK73" s="0">
-        <v>26177.6742081448</v>
+        <v>2.61776742081448</v>
       </c>
       <c r="AL73" s="0">
         <v>3656.06557377049</v>
@@ -14822,7 +14822,7 @@
         <v>10039.4824120603</v>
       </c>
       <c r="AK74" s="0">
-        <v>4964.77822580645</v>
+        <v>0.496477822580645</v>
       </c>
       <c r="AL74" s="0">
         <v>2708.03038674033</v>
@@ -15017,7 +15017,7 @@
         <v>17651.4117647059</v>
       </c>
       <c r="AK75" s="0">
-        <v>10512.5909090909</v>
+        <v>1.05125909090909</v>
       </c>
       <c r="AL75" s="0">
         <v>13581.4814814815</v>
@@ -15212,7 +15212,7 @@
         <v>12729.7183098592</v>
       </c>
       <c r="AK76" s="0">
-        <v>8107.27272727273</v>
+        <v>0.810727272727273</v>
       </c>
       <c r="AL76" s="0">
         <v>1263.39603960396</v>
@@ -15407,7 +15407,7 @@
         <v>72472.4545454545</v>
       </c>
       <c r="AK77" s="0">
-        <v>31113.519379845</v>
+        <v>3.1113519379845</v>
       </c>
       <c r="AL77" s="0">
         <v>20922.0238095238</v>
@@ -15602,7 +15602,7 @@
         <v>19025.5416666667</v>
       </c>
       <c r="AK78" s="0">
-        <v>9349.82142857143</v>
+        <v>0.934982142857143</v>
       </c>
       <c r="AL78" s="0">
         <v>1458.57142857143</v>
@@ -15797,7 +15797,7 @@
         <v>25409.9705882353</v>
       </c>
       <c r="AK79" s="0">
-        <v>17047.4630872483</v>
+        <v>1.70474630872483</v>
       </c>
       <c r="AL79" s="0">
         <v>3209.62121212121</v>
@@ -15992,7 +15992,7 @@
         <v>15926.1515151515</v>
       </c>
       <c r="AK80" s="0">
-        <v>10358.5491803279</v>
+        <v>1.03585491803279</v>
       </c>
       <c r="AL80" s="0">
         <v>866.666666666667</v>
@@ -16187,7 +16187,7 @@
         <v>49323.1182795699</v>
       </c>
       <c r="AK81" s="0">
-        <v>27425.1639344262</v>
+        <v>2.74251639344262</v>
       </c>
       <c r="AL81" s="0">
         <v>12969.012345679</v>
@@ -16382,7 +16382,7 @@
         <v>24181.1470588235</v>
       </c>
       <c r="AK82" s="0">
-        <v>12398.9875</v>
+        <v>1.23989875</v>
       </c>
       <c r="AL82" s="0">
         <v>4078.26086956522</v>
@@ -16577,7 +16577,7 @@
         <v>19752.675</v>
       </c>
       <c r="AK83" s="0">
-        <v>13794.4863725142</v>
+        <v>1.37944863725142</v>
       </c>
       <c r="AL83" s="0">
         <v>7045.2</v>
@@ -16772,7 +16772,7 @@
         <v>27152.6632653061</v>
       </c>
       <c r="AK84" s="0">
-        <v>22882.787037037</v>
+        <v>2.2882787037037</v>
       </c>
       <c r="AL84" s="0">
         <v>1222.44</v>
@@ -16967,7 +16967,7 @@
         <v>39200.12</v>
       </c>
       <c r="AK85" s="0">
-        <v>19275.4603174603</v>
+        <v>1.92754603174603</v>
       </c>
       <c r="AL85" s="0">
         <v>2650.97142857143</v>
@@ -17162,7 +17162,7 @@
         <v>44045.55</v>
       </c>
       <c r="AK86" s="0">
-        <v>21608.5714285714</v>
+        <v>2.16085714285714</v>
       </c>
       <c r="AL86" s="0">
         <v>7008.51063829787</v>
@@ -17357,7 +17357,7 @@
         <v>101946.333333333</v>
       </c>
       <c r="AK87" s="0">
-        <v>57617.2399823589</v>
+        <v>5.76172399823589</v>
       </c>
       <c r="AL87" s="0">
         <v>11700</v>
@@ -17552,7 +17552,7 @@
         <v>9700.95833333333</v>
       </c>
       <c r="AK88" s="0">
-        <v>5397.13385826772</v>
+        <v>0.539713385826772</v>
       </c>
       <c r="AL88" s="0">
         <v>2030.42352941176</v>
@@ -17747,7 +17747,7 @@
         <v>28328.7684729064</v>
       </c>
       <c r="AK89" s="0">
-        <v>14473.7168141593</v>
+        <v>1.44737168141593</v>
       </c>
       <c r="AL89" s="0">
         <v>9288.58682634731</v>
@@ -17942,7 +17942,7 @@
         <v>55713.75</v>
       </c>
       <c r="AK90" s="0">
-        <v>45391.0714285714</v>
+        <v>4.53910714285714</v>
       </c>
       <c r="AL90" s="0">
         <v>2591.5625</v>
@@ -18137,7 +18137,7 @@
         <v>29322.6091954023</v>
       </c>
       <c r="AK91" s="0">
-        <v>18253.1957446809</v>
+        <v>1.82531957446809</v>
       </c>
       <c r="AL91" s="0">
         <v>2325.43609022556</v>
@@ -18332,7 +18332,7 @@
         <v>25195.1817103795</v>
       </c>
       <c r="AK92" s="0">
-        <v>13203.3150140571</v>
+        <v>1.32033150140571</v>
       </c>
       <c r="AL92" s="0">
         <v>4059.65714285714</v>
@@ -18527,7 +18527,7 @@
         <v>59268.6896551724</v>
       </c>
       <c r="AK93" s="0">
-        <v>29035.7967479675</v>
+        <v>2.90357967479675</v>
       </c>
       <c r="AL93" s="0">
         <v>18119.875</v>
@@ -18722,7 +18722,7 @@
         <v>24187.7731958763</v>
       </c>
       <c r="AK94" s="0">
-        <v>13652.9380530973</v>
+        <v>1.36529380530973</v>
       </c>
       <c r="AL94" s="0">
         <v>11534.1333333333</v>
@@ -18917,7 +18917,7 @@
         <v>16066.1111111111</v>
       </c>
       <c r="AK95" s="0">
-        <v>13387.5539568345</v>
+        <v>1.33875539568345</v>
       </c>
       <c r="AL95" s="0">
         <v>3690.76923076923</v>
@@ -19112,7 +19112,7 @@
         <v>46685.6857142857</v>
       </c>
       <c r="AK96" s="0">
-        <v>23196.8217054264</v>
+        <v>2.31968217054264</v>
       </c>
       <c r="AL96" s="0">
         <v>8086.32926829268</v>
@@ -19307,7 +19307,7 @@
         <v>38775.9432624113</v>
       </c>
       <c r="AK97" s="0">
-        <v>25475.8363351422</v>
+        <v>2.54758363351422</v>
       </c>
       <c r="AL97" s="0">
         <v>4025.67796610169</v>
@@ -19502,7 +19502,7 @@
         <v>88200.8275862069</v>
       </c>
       <c r="AK98" s="0">
-        <v>47985.1898734177</v>
+        <v>4.79851898734177</v>
       </c>
       <c r="AL98" s="0">
         <v>1580</v>
@@ -19697,7 +19697,7 @@
         <v>27011.9836065574</v>
       </c>
       <c r="AK99" s="0">
-        <v>14289.2602739726</v>
+        <v>1.42892602739726</v>
       </c>
       <c r="AL99" s="0">
         <v>1521.10091743119</v>
@@ -19892,7 +19892,7 @@
         <v>38214.4392361111</v>
       </c>
       <c r="AK100" s="0">
-        <v>22425.9291901203</v>
+        <v>2.24259291901203</v>
       </c>
       <c r="AL100" s="0">
         <v>4052.63157894737</v>
@@ -20087,7 +20087,7 @@
         <v>20939.1239669421</v>
       </c>
       <c r="AK101" s="0">
-        <v>14583.5602836879</v>
+        <v>1.45835602836879</v>
       </c>
       <c r="AL101" s="0">
         <v>4129.69696969697</v>
@@ -20282,7 +20282,7 @@
         <v>22439.4404761905</v>
       </c>
       <c r="AK102" s="0">
-        <v>6872.57943925234</v>
+        <v>0.687257943925234</v>
       </c>
       <c r="AL102" s="0">
         <v>50029.0625</v>
@@ -20477,7 +20477,7 @@
         <v>19433.7471264368</v>
       </c>
       <c r="AK103" s="0">
-        <v>11359.9015544041</v>
+        <v>1.13599015544041</v>
       </c>
       <c r="AL103" s="0">
         <v>2364.89655172414</v>
@@ -20672,7 +20672,7 @@
         <v>22579.7288135593</v>
       </c>
       <c r="AK104" s="0">
-        <v>15191.5905511811</v>
+        <v>1.51915905511811</v>
       </c>
       <c r="AL104" s="0">
         <v>613.114754098361</v>
@@ -20867,7 +20867,7 @@
         <v>26165.1772727273</v>
       </c>
       <c r="AK105" s="0">
-        <v>13675.417721519</v>
+        <v>1.3675417721519</v>
       </c>
       <c r="AL105" s="0">
         <v>6920.75757575758</v>
@@ -21062,7 +21062,7 @@
         <v>39956.25</v>
       </c>
       <c r="AK106" s="0">
-        <v>21478.2647058824</v>
+        <v>2.14782647058824</v>
       </c>
       <c r="AL106" s="0">
         <v>10689.9322033898</v>
@@ -21257,7 +21257,7 @@
         <v>20216.7692307692</v>
       </c>
       <c r="AK107" s="0">
-        <v>15390.0934579439</v>
+        <v>1.53900934579439</v>
       </c>
       <c r="AL107" s="0">
         <v>5504</v>
@@ -21452,7 +21452,7 @@
         <v>35935.9066666667</v>
       </c>
       <c r="AK108" s="0">
-        <v>21736.956043956</v>
+        <v>2.1736956043956</v>
       </c>
       <c r="AL108" s="0">
         <v>8937.85087719298</v>
@@ -21647,7 +21647,7 @@
         <v>42559.8421052632</v>
       </c>
       <c r="AK109" s="0">
-        <v>26616.6458333333</v>
+        <v>2.66166458333333</v>
       </c>
       <c r="AL109" s="0">
         <v>6965.15217391304</v>
@@ -21842,7 +21842,7 @@
         <v>14648.5669291339</v>
       </c>
       <c r="AK110" s="0">
-        <v>7280.18309859155</v>
+        <v>0.728018309859155</v>
       </c>
       <c r="AL110" s="0">
         <v>3460.43956043956</v>
@@ -22037,7 +22037,7 @@
         <v>33583.8492462312</v>
       </c>
       <c r="AK111" s="0">
-        <v>22060.3146551724</v>
+        <v>2.20603146551724</v>
       </c>
       <c r="AL111" s="0">
         <v>8011.97350993377</v>
@@ -22232,7 +22232,7 @@
         <v>36118.9591836735</v>
       </c>
       <c r="AK112" s="0">
-        <v>29718.5636363636</v>
+        <v>2.97185636363636</v>
       </c>
       <c r="AL112" s="0">
         <v>2407.32394366197</v>
@@ -22427,7 +22427,7 @@
         <v>22284.7244897959</v>
       </c>
       <c r="AK113" s="0">
-        <v>11970.525</v>
+        <v>1.1970525</v>
       </c>
       <c r="AL113" s="0">
         <v>2004.21052631579</v>
@@ -22622,7 +22622,7 @@
         <v>27420.5299145299</v>
       </c>
       <c r="AK114" s="0">
-        <v>11378.5267175573</v>
+        <v>1.13785267175573</v>
       </c>
       <c r="AL114" s="0">
         <v>5950.93975903615</v>
@@ -22817,7 +22817,7 @@
         <v>49030.937037037</v>
       </c>
       <c r="AK115" s="0">
-        <v>38489.0396039604</v>
+        <v>3.84890396039604</v>
       </c>
       <c r="AL115" s="0">
         <v>2565.93922651934</v>
@@ -23012,7 +23012,7 @@
         <v>50933.1460674157</v>
       </c>
       <c r="AK116" s="0">
-        <v>32886.5</v>
+        <v>3.28865</v>
       </c>
       <c r="AL116" s="0">
         <v>18473.2142857143</v>
@@ -23207,7 +23207,7 @@
         <v>27711.2696707589</v>
       </c>
       <c r="AK117" s="0">
-        <v>15930.1131752665</v>
+        <v>1.59301131752665</v>
       </c>
       <c r="AL117" s="0">
         <v>5855.59139784946</v>
@@ -23402,7 +23402,7 @@
         <v>31359.78125</v>
       </c>
       <c r="AK118" s="0">
-        <v>15470.6857142857</v>
+        <v>1.54706857142857</v>
       </c>
       <c r="AL118" s="0">
         <v>1391.70149253731</v>
@@ -23597,7 +23597,7 @@
         <v>44894.4615384615</v>
       </c>
       <c r="AK119" s="0">
-        <v>34211.4962962963</v>
+        <v>3.42114962962963</v>
       </c>
       <c r="AL119" s="0">
         <v>44326.0759493671</v>
@@ -23792,7 +23792,7 @@
         <v>18441.3377483444</v>
       </c>
       <c r="AK120" s="0">
-        <v>11855.2371794872</v>
+        <v>1.18552371794872</v>
       </c>
       <c r="AL120" s="0">
         <v>10642.8571428571</v>
@@ -23987,7 +23987,7 @@
         <v>19055.9863013699</v>
       </c>
       <c r="AK121" s="0">
-        <v>12030.2317073171</v>
+        <v>1.20302317073171</v>
       </c>
       <c r="AL121" s="0">
         <v>2035.0303030303</v>
@@ -24182,7 +24182,7 @@
         <v>57174.6104403409</v>
       </c>
       <c r="AK122" s="0">
-        <v>31337.4743111165</v>
+        <v>3.13374743111165</v>
       </c>
       <c r="AL122" s="0">
         <v>2813.6170212766</v>
@@ -24377,7 +24377,7 @@
         <v>20302.5204081633</v>
       </c>
       <c r="AK123" s="0">
-        <v>12689.0865800866</v>
+        <v>1.26890865800866</v>
       </c>
       <c r="AL123" s="0">
         <v>4245.21472392638</v>
@@ -24572,7 +24572,7 @@
         <v>23009.2340099299</v>
       </c>
       <c r="AK124" s="0">
-        <v>12741.8354900521</v>
+        <v>1.27418354900521</v>
       </c>
       <c r="AL124" s="0">
         <v>3932.63157894737</v>
@@ -24767,7 +24767,7 @@
         <v>14323.5744305541</v>
       </c>
       <c r="AK125" s="0">
-        <v>7850.37555252878</v>
+        <v>0.785037555252878</v>
       </c>
       <c r="AL125" s="0">
         <v>1768.29927007299</v>
@@ -24962,7 +24962,7 @@
         <v>25335.0553588867</v>
       </c>
       <c r="AK126" s="0">
-        <v>16330.5183622941</v>
+        <v>1.63305183622941</v>
       </c>
       <c r="AL126" s="0">
         <v>8171.20879120879</v>
@@ -25157,7 +25157,7 @@
         <v>26799.1428571429</v>
       </c>
       <c r="AK127" s="0">
-        <v>16714.6126760563</v>
+        <v>1.67146126760563</v>
       </c>
       <c r="AL127" s="0">
         <v>3235.20408163265</v>
@@ -25352,7 +25352,7 @@
         <v>43753.6896551724</v>
       </c>
       <c r="AK128" s="0">
-        <v>23789.5384615385</v>
+        <v>2.37895384615385</v>
       </c>
       <c r="AL128" s="0">
         <v>3632.29508196721</v>
@@ -25547,7 +25547,7 @@
         <v>22732.328358209</v>
       </c>
       <c r="AK129" s="0">
-        <v>11025.734939759</v>
+        <v>1.1025734939759</v>
       </c>
       <c r="AL129" s="0">
         <v>9528.52941176471</v>
@@ -25742,7 +25742,7 @@
         <v>17938.32</v>
       </c>
       <c r="AK130" s="0">
-        <v>11204.476744186</v>
+        <v>1.1204476744186</v>
       </c>
       <c r="AL130" s="0">
         <v>5797.12</v>
@@ -25937,7 +25937,7 @@
         <v>16460.9489795918</v>
       </c>
       <c r="AK131" s="0">
-        <v>9945.9037037037</v>
+        <v>0.99459037037037</v>
       </c>
       <c r="AL131" s="0">
         <v>1897.61904761905</v>
@@ -26132,7 +26132,7 @@
         <v>24374.5784313725</v>
       </c>
       <c r="AK132" s="0">
-        <v>13953.8383838384</v>
+        <v>1.39538383838384</v>
       </c>
       <c r="AL132" s="0">
         <v>5159.24347826087</v>
@@ -26327,7 +26327,7 @@
         <v>22773.2941176471</v>
       </c>
       <c r="AK133" s="0">
-        <v>14293.1092436975</v>
+        <v>1.42931092436975</v>
       </c>
       <c r="AL133" s="0">
         <v>4808.72093023256</v>
@@ -26522,7 +26522,7 @@
         <v>49048.5111111111</v>
       </c>
       <c r="AK134" s="0">
-        <v>25414.5230744191</v>
+        <v>2.54145230744191</v>
       </c>
       <c r="AL134" s="0">
         <v>225.478260869565</v>
@@ -26717,7 +26717,7 @@
         <v>101840.1</v>
       </c>
       <c r="AK135" s="0">
-        <v>63162.1666666667</v>
+        <v>6.31621666666667</v>
       </c>
       <c r="AL135" s="0">
         <v>1900</v>
@@ -26912,7 +26912,7 @@
         <v>54953.6888888889</v>
       </c>
       <c r="AK136" s="0">
-        <v>32730.7222222222</v>
+        <v>3.27307222222222</v>
       </c>
       <c r="AL136" s="0">
         <v>1762.5</v>
@@ -27107,7 +27107,7 @@
         <v>14098.3440860215</v>
       </c>
       <c r="AK137" s="0">
-        <v>9168.29577464789</v>
+        <v>0.916829577464789</v>
       </c>
       <c r="AL137" s="0">
         <v>3368.9247311828</v>
@@ -27302,7 +27302,7 @@
         <v>34301.0769230769</v>
       </c>
       <c r="AK138" s="0">
-        <v>22772.2372881356</v>
+        <v>2.27722372881356</v>
       </c>
       <c r="AL138" s="0">
         <v>3852.38095238095</v>
@@ -27497,7 +27497,7 @@
         <v>47289.4473684211</v>
       </c>
       <c r="AK139" s="0">
-        <v>25953.5684210526</v>
+        <v>2.59535684210526</v>
       </c>
       <c r="AL139" s="0">
         <v>9914.17721518987</v>
@@ -27692,7 +27692,7 @@
         <v>52705.5531914894</v>
       </c>
       <c r="AK140" s="0">
-        <v>20692.1547619048</v>
+        <v>2.06921547619048</v>
       </c>
       <c r="AL140" s="0">
         <v>25728.8</v>
@@ -27887,7 +27887,7 @@
         <v>22100.5222222222</v>
       </c>
       <c r="AK141" s="0">
-        <v>13825.2410714286</v>
+        <v>1.38252410714286</v>
       </c>
       <c r="AL141" s="0">
         <v>5917.02127659574</v>
@@ -28082,7 +28082,7 @@
         <v>45453.4255319149</v>
       </c>
       <c r="AK142" s="0">
-        <v>25456.661971831</v>
+        <v>2.5456661971831</v>
       </c>
       <c r="AL142" s="0">
         <v>5163.26530612245</v>
@@ -28277,7 +28277,7 @@
         <v>8011.75</v>
       </c>
       <c r="AK143" s="0">
-        <v>3542.91111111111</v>
+        <v>0.354291111111111</v>
       </c>
       <c r="AL143" s="0">
         <v>1904.61538461538</v>
@@ -28472,7 +28472,7 @@
         <v>34601.7446073009</v>
       </c>
       <c r="AK144" s="0">
-        <v>22806.5029537577</v>
+        <v>2.28065029537577</v>
       </c>
       <c r="AL144" s="0">
         <v>3019.05737704918</v>
@@ -28667,7 +28667,7 @@
         <v>30809.9879518072</v>
       </c>
       <c r="AK145" s="0">
-        <v>19039.6377952756</v>
+        <v>1.90396377952756</v>
       </c>
       <c r="AL145" s="0">
         <v>2920.96774193548</v>
@@ -28862,7 +28862,7 @@
         <v>35740.0454545455</v>
       </c>
       <c r="AK146" s="0">
-        <v>20265.3859649123</v>
+        <v>2.02653859649123</v>
       </c>
       <c r="AL146" s="0">
         <v>4459.13978494624</v>
@@ -29057,7 +29057,7 @@
         <v>14654.8097560976</v>
       </c>
       <c r="AK147" s="0">
-        <v>8361.97265625</v>
+        <v>0.836197265625</v>
       </c>
       <c r="AL147" s="0">
         <v>3538.94859813084</v>
@@ -29252,7 +29252,7 @@
         <v>22051.28</v>
       </c>
       <c r="AK148" s="0">
-        <v>13944.6769230769</v>
+        <v>1.39446769230769</v>
       </c>
       <c r="AL148" s="0">
         <v>4830.94339622641</v>
@@ -29447,7 +29447,7 @@
         <v>27019.6666666667</v>
       </c>
       <c r="AK149" s="0">
-        <v>16762.8387096774</v>
+        <v>1.67628387096774</v>
       </c>
       <c r="AL149" s="0">
         <v>8615.74468085106</v>
@@ -29642,7 +29642,7 @@
         <v>21986.5277777778</v>
       </c>
       <c r="AK150" s="0">
-        <v>9753.36734693878</v>
+        <v>0.975336734693878</v>
       </c>
       <c r="AL150" s="0">
         <v>8034.8051948052</v>
@@ -29837,7 +29837,7 @@
         <v>25897.0361445783</v>
       </c>
       <c r="AK151" s="0">
-        <v>17904</v>
+        <v>1.7904</v>
       </c>
       <c r="AL151" s="0">
         <v>2753.64705882353</v>
@@ -30032,7 +30032,7 @@
         <v>63103.8787878788</v>
       </c>
       <c r="AK152" s="0">
-        <v>31553.2837837838</v>
+        <v>3.15532837837838</v>
       </c>
       <c r="AL152" s="0">
         <v>18582.8571428571</v>
@@ -30227,7 +30227,7 @@
         <v>35813.7101449275</v>
       </c>
       <c r="AK153" s="0">
-        <v>37261.5208333333</v>
+        <v>3.72615208333333</v>
       </c>
       <c r="AL153" s="0">
         <v>399.915492957746</v>
@@ -30422,7 +30422,7 @@
         <v>25735.0980392157</v>
       </c>
       <c r="AK154" s="0">
-        <v>9744.20338983051</v>
+        <v>0.974420338983051</v>
       </c>
       <c r="AL154" s="0">
         <v>11581.5825242718</v>
@@ -30617,7 +30617,7 @@
         <v>12748.4186046512</v>
       </c>
       <c r="AK155" s="0">
-        <v>6660.15</v>
+        <v>0.666015</v>
       </c>
       <c r="AL155" s="0">
         <v>4687.7358490566</v>
@@ -30812,7 +30812,7 @@
         <v>29144.8767123288</v>
       </c>
       <c r="AK156" s="0">
-        <v>19627.3759398496</v>
+        <v>1.96273759398496</v>
       </c>
       <c r="AL156" s="0">
         <v>4190</v>
@@ -31007,7 +31007,7 @@
         <v>19744.2470327524</v>
       </c>
       <c r="AK157" s="0">
-        <v>14035.7589089134</v>
+        <v>1.40357589089134</v>
       </c>
       <c r="AL157" s="0">
         <v>2010</v>
@@ -31202,7 +31202,7 @@
         <v>35957.4509803922</v>
       </c>
       <c r="AK158" s="0">
-        <v>25193.4615384615</v>
+        <v>2.51934615384615</v>
       </c>
       <c r="AL158" s="0">
         <v>1398.59649122807</v>
@@ -31397,7 +31397,7 @@
         <v>61506.7619047619</v>
       </c>
       <c r="AK159" s="0">
-        <v>37485.4478845731</v>
+        <v>3.74854478845731</v>
       </c>
       <c r="AL159" s="0">
         <v>4004.34782608696</v>
@@ -31592,7 +31592,7 @@
         <v>60805.7142857143</v>
       </c>
       <c r="AK160" s="0">
-        <v>34982.9565217391</v>
+        <v>3.49829565217391</v>
       </c>
       <c r="AL160" s="0">
         <v>2500</v>
@@ -31787,7 +31787,7 @@
         <v>48411.125</v>
       </c>
       <c r="AK161" s="0">
-        <v>27158.6153846154</v>
+        <v>2.71586153846154</v>
       </c>
       <c r="AL161" s="0">
         <v>3125</v>
@@ -31982,7 +31982,7 @@
         <v>26551.1428571429</v>
       </c>
       <c r="AK162" s="0">
-        <v>16423.8088235294</v>
+        <v>1.64238088235294</v>
       </c>
       <c r="AL162" s="0">
         <v>6239.39316239316</v>
@@ -32177,7 +32177,7 @@
         <v>23999.0588235294</v>
       </c>
       <c r="AK163" s="0">
-        <v>18373.9603960396</v>
+        <v>1.83739603960396</v>
       </c>
       <c r="AL163" s="0">
         <v>2855.39682539683</v>
@@ -32372,7 +32372,7 @@
         <v>109785.244357639</v>
       </c>
       <c r="AK164" s="0">
-        <v>61758.7199991862</v>
+        <v>6.17587199991862</v>
       </c>
       <c r="AL164" s="0">
         <v>6564.10256410256</v>
@@ -32567,7 +32567,7 @@
         <v>18451.7222222222</v>
       </c>
       <c r="AK165" s="0">
-        <v>13750.3482142857</v>
+        <v>1.37503482142857</v>
       </c>
       <c r="AL165" s="0">
         <v>3234.63414634146</v>
@@ -32762,7 +32762,7 @@
         <v>94209.696969697</v>
       </c>
       <c r="AK166" s="0">
-        <v>52444</v>
+        <v>5.2444</v>
       </c>
       <c r="AL166" s="0">
         <v>13594.4444444444</v>
@@ -32957,7 +32957,7 @@
         <v>27340.9961389961</v>
       </c>
       <c r="AK167" s="0">
-        <v>12856.6300614246</v>
+        <v>1.28566300614246</v>
       </c>
       <c r="AL167" s="0">
         <v>9123.6015037594</v>
@@ -33152,7 +33152,7 @@
         <v>65836.3333333333</v>
       </c>
       <c r="AK168" s="0">
-        <v>43427.606557377</v>
+        <v>4.3427606557377</v>
       </c>
       <c r="AL168" s="0">
         <v>6995.12195121951</v>
@@ -33347,7 +33347,7 @@
         <v>24356.6933333333</v>
       </c>
       <c r="AK169" s="0">
-        <v>11828.797979798</v>
+        <v>1.1828797979798</v>
       </c>
       <c r="AL169" s="0">
         <v>6956.34146341463</v>
@@ -33542,7 +33542,7 @@
         <v>24488.0400010851</v>
       </c>
       <c r="AK170" s="0">
-        <v>17146.4895522274</v>
+        <v>1.71464895522274</v>
       </c>
       <c r="AL170" s="0">
         <v>4267.96116504854</v>
@@ -33737,7 +33737,7 @@
         <v>26725.1034482759</v>
       </c>
       <c r="AK171" s="0">
-        <v>10283.2421052632</v>
+        <v>1.02832421052632</v>
       </c>
       <c r="AL171" s="0">
         <v>10403.1746031746</v>
@@ -33932,7 +33932,7 @@
         <v>69992.8125</v>
       </c>
       <c r="AK172" s="0">
-        <v>39533.9215686274</v>
+        <v>3.95339215686274</v>
       </c>
       <c r="AL172" s="0">
         <v>402.941176470588</v>
@@ -34127,7 +34127,7 @@
         <v>49793.8769230769</v>
       </c>
       <c r="AK173" s="0">
-        <v>25950.9391576943</v>
+        <v>2.59509391576943</v>
       </c>
       <c r="AL173" s="0">
         <v>2363.07692307692</v>
@@ -34322,7 +34322,7 @@
         <v>43575.7171959005</v>
       </c>
       <c r="AK174" s="0">
-        <v>23254.0016965704</v>
+        <v>2.32540016965704</v>
       </c>
       <c r="AL174" s="0">
         <v>8337.0101010101</v>
@@ -34517,7 +34517,7 @@
         <v>102209</v>
       </c>
       <c r="AK175" s="0">
-        <v>51236.625</v>
+        <v>5.1236625</v>
       </c>
       <c r="AL175" s="0">
         <v>31200</v>
@@ -34712,7 +34712,7 @@
         <v>67056.8421052632</v>
       </c>
       <c r="AK176" s="0">
-        <v>30947.3684210526</v>
+        <v>3.09473684210526</v>
       </c>
       <c r="AL176" s="0">
         <v>17705.2631578947</v>
@@ -34907,7 +34907,7 @@
         <v>30562.8518518519</v>
       </c>
       <c r="AK177" s="0">
-        <v>17510.4015151515</v>
+        <v>1.75104015151515</v>
       </c>
       <c r="AL177" s="0">
         <v>-1406.66666666667</v>
@@ -35102,7 +35102,7 @@
         <v>29931.8902420343</v>
       </c>
       <c r="AK178" s="0">
-        <v>19638.2530300256</v>
+        <v>1.96382530300256</v>
       </c>
       <c r="AL178" s="0">
         <v>3663.39285714286</v>
@@ -35297,7 +35297,7 @@
         <v>23932.505050505</v>
       </c>
       <c r="AK179" s="0">
-        <v>13881.606557377</v>
+        <v>1.3881606557377</v>
       </c>
       <c r="AL179" s="0">
         <v>3884.74747474747</v>
@@ -35492,7 +35492,7 @@
         <v>53244.6689814815</v>
       </c>
       <c r="AK180" s="0">
-        <v>27698.1225585938</v>
+        <v>2.76981225585938</v>
       </c>
       <c r="AL180" s="0">
         <v>9639.73684210526</v>
@@ -35687,7 +35687,7 @@
         <v>42997.1555555556</v>
       </c>
       <c r="AK181" s="0">
-        <v>25830.03125</v>
+        <v>2.583003125</v>
       </c>
       <c r="AL181" s="0">
         <v>4777.55102040816</v>
@@ -35882,7 +35882,7 @@
         <v>50106.4285714286</v>
       </c>
       <c r="AK182" s="0">
-        <v>31154.4623655914</v>
+        <v>3.11544623655914</v>
       </c>
       <c r="AL182" s="0">
         <v>16883.6111111111</v>
@@ -36077,7 +36077,7 @@
         <v>33961.7016129032</v>
       </c>
       <c r="AK183" s="0">
-        <v>25408.3063583815</v>
+        <v>2.54083063583815</v>
       </c>
       <c r="AL183" s="0">
         <v>4786.9696969697</v>
@@ -36272,7 +36272,7 @@
         <v>38579.6363636364</v>
       </c>
       <c r="AK184" s="0">
-        <v>33777.0909090909</v>
+        <v>3.37770909090909</v>
       </c>
       <c r="AL184" s="0">
         <v>0</v>
@@ -36467,7 +36467,7 @@
         <v>13468.9411764706</v>
       </c>
       <c r="AK185" s="0">
-        <v>5397.85869565217</v>
+        <v>0.539785869565217</v>
       </c>
       <c r="AL185" s="0">
         <v>3566.27450980392</v>
@@ -36662,7 +36662,7 @@
         <v>41722.5479452055</v>
       </c>
       <c r="AK186" s="0">
-        <v>22134.1</v>
+        <v>2.21341</v>
       </c>
       <c r="AL186" s="0">
         <v>8845.98734177215</v>
@@ -36857,7 +36857,7 @@
         <v>17516.3611111111</v>
       </c>
       <c r="AK187" s="0">
-        <v>9127.73109243697</v>
+        <v>0.912773109243697</v>
       </c>
       <c r="AL187" s="0">
         <v>2152</v>
@@ -37052,7 +37052,7 @@
         <v>36306.2888888889</v>
       </c>
       <c r="AK188" s="0">
-        <v>22457.1447368421</v>
+        <v>2.24571447368421</v>
       </c>
       <c r="AL188" s="0">
         <v>8461.98412698413</v>
@@ -37247,7 +37247,7 @@
         <v>16083.6666666667</v>
       </c>
       <c r="AK189" s="0">
-        <v>10361.4302325581</v>
+        <v>1.03614302325581</v>
       </c>
       <c r="AL189" s="0">
         <v>1720.91503267974</v>
@@ -37442,7 +37442,7 @@
         <v>37657.4461538462</v>
       </c>
       <c r="AK190" s="0">
-        <v>22362.4395604396</v>
+        <v>2.23624395604396</v>
       </c>
       <c r="AL190" s="0">
         <v>4645.85714285714</v>
@@ -37637,7 +37637,7 @@
         <v>31273.70796875</v>
       </c>
       <c r="AK191" s="0">
-        <v>18114.1402984164</v>
+        <v>1.81141402984164</v>
       </c>
       <c r="AL191" s="0">
         <v>4668.28828828829</v>
@@ -37832,7 +37832,7 @@
         <v>21146.3888888889</v>
       </c>
       <c r="AK192" s="0">
-        <v>13071.7222222222</v>
+        <v>1.30717222222222</v>
       </c>
       <c r="AL192" s="0">
         <v>3166.88372093023</v>
@@ -38027,7 +38027,7 @@
         <v>10217.3033707865</v>
       </c>
       <c r="AK193" s="0">
-        <v>4439.88679245283</v>
+        <v>0.443988679245283</v>
       </c>
       <c r="AL193" s="0">
         <v>5851.64835164835</v>
@@ -38222,7 +38222,7 @@
         <v>36372.275862069</v>
       </c>
       <c r="AK194" s="0">
-        <v>21789.3193277311</v>
+        <v>2.17893193277311</v>
       </c>
       <c r="AL194" s="0">
         <v>6764.36781609195</v>
@@ -38417,7 +38417,7 @@
         <v>33267.4287109375</v>
       </c>
       <c r="AK195" s="0">
-        <v>21879.1214453125</v>
+        <v>2.18791214453125</v>
       </c>
       <c r="AL195" s="0">
         <v>2750.30769230769</v>
@@ -38612,7 +38612,7 @@
         <v>31503.3913043478</v>
       </c>
       <c r="AK196" s="0">
-        <v>19863.1185770751</v>
+        <v>1.98631185770751</v>
       </c>
       <c r="AL196" s="0">
         <v>5155.78010471204</v>
@@ -38807,7 +38807,7 @@
         <v>35524.8602150538</v>
       </c>
       <c r="AK197" s="0">
-        <v>21193.9908256881</v>
+        <v>2.11939908256881</v>
       </c>
       <c r="AL197" s="0">
         <v>5931.49473684211</v>
@@ -39002,7 +39002,7 @@
         <v>23294.3684210526</v>
       </c>
       <c r="AK198" s="0">
-        <v>13435.3854166667</v>
+        <v>1.34353854166667</v>
       </c>
       <c r="AL198" s="0">
         <v>6562.55</v>
@@ -39197,7 +39197,7 @@
         <v>54692.3050847458</v>
       </c>
       <c r="AK199" s="0">
-        <v>33241.3987730061</v>
+        <v>3.32413987730061</v>
       </c>
       <c r="AL199" s="0">
         <v>3656.06557377049</v>
@@ -39392,7 +39392,7 @@
         <v>13055.6903409091</v>
       </c>
       <c r="AK200" s="0">
-        <v>7038.69266055046</v>
+        <v>0.703869266055046</v>
       </c>
       <c r="AL200" s="0">
         <v>2708.03038674033</v>
@@ -39587,7 +39587,7 @@
         <v>46415.44</v>
       </c>
       <c r="AK201" s="0">
-        <v>22522.1428571429</v>
+        <v>2.25221428571429</v>
       </c>
       <c r="AL201" s="0">
         <v>13581.4814814815</v>
@@ -39782,7 +39782,7 @@
         <v>11475.6489361702</v>
       </c>
       <c r="AK202" s="0">
-        <v>6261.14705882353</v>
+        <v>0.626114705882353</v>
       </c>
       <c r="AL202" s="0">
         <v>1263.39603960396</v>
@@ -39977,7 +39977,7 @@
         <v>63067.6097560976</v>
       </c>
       <c r="AK203" s="0">
-        <v>33515.724137931</v>
+        <v>3.3515724137931</v>
       </c>
       <c r="AL203" s="0">
         <v>20922.0238095238</v>
@@ -40172,7 +40172,7 @@
         <v>16200.0615384615</v>
       </c>
       <c r="AK204" s="0">
-        <v>8299.30973451327</v>
+        <v>0.829930973451327</v>
       </c>
       <c r="AL204" s="0">
         <v>1458.57142857143</v>
@@ -40367,7 +40367,7 @@
         <v>25064.7175572519</v>
       </c>
       <c r="AK205" s="0">
-        <v>16255.5611510791</v>
+        <v>1.62555611510791</v>
       </c>
       <c r="AL205" s="0">
         <v>3209.62121212121</v>
@@ -40562,7 +40562,7 @@
         <v>17087.0133333333</v>
       </c>
       <c r="AK206" s="0">
-        <v>12263.4174757282</v>
+        <v>1.22634174757282</v>
       </c>
       <c r="AL206" s="0">
         <v>866.666666666667</v>
@@ -40757,7 +40757,7 @@
         <v>46155.3768115942</v>
       </c>
       <c r="AK207" s="0">
-        <v>27746.5333333333</v>
+        <v>2.77465333333333</v>
       </c>
       <c r="AL207" s="0">
         <v>12969.012345679</v>
@@ -40952,7 +40952,7 @@
         <v>34621.4347826087</v>
       </c>
       <c r="AK208" s="0">
-        <v>22353.0169491525</v>
+        <v>2.23530169491525</v>
       </c>
       <c r="AL208" s="0">
         <v>4078.26086956522</v>
@@ -41147,7 +41147,7 @@
         <v>25400.8</v>
       </c>
       <c r="AK209" s="0">
-        <v>19324.4035213695</v>
+        <v>1.93244035213695</v>
       </c>
       <c r="AL209" s="0">
         <v>7045.2</v>
@@ -41342,7 +41342,7 @@
         <v>11691.3492930238</v>
       </c>
       <c r="AK210" s="0">
-        <v>7702.52000054253</v>
+        <v>0.770252000054254</v>
       </c>
       <c r="AL210" s="0">
         <v>1222.44</v>
@@ -41537,7 +41537,7 @@
         <v>40730.3529411765</v>
       </c>
       <c r="AK211" s="0">
-        <v>22453</v>
+        <v>2.2453</v>
       </c>
       <c r="AL211" s="0">
         <v>2650.97142857143</v>
@@ -41732,7 +41732,7 @@
         <v>38647.8222222222</v>
       </c>
       <c r="AK212" s="0">
-        <v>24076.619047619</v>
+        <v>2.4076619047619</v>
       </c>
       <c r="AL212" s="0">
         <v>7008.51063829787</v>
@@ -41927,7 +41927,7 @@
         <v>107620</v>
       </c>
       <c r="AK213" s="0">
-        <v>92395.1063829787</v>
+        <v>9.23951063829787</v>
       </c>
       <c r="AL213" s="0">
         <v>11700</v>
@@ -42122,7 +42122,7 @@
         <v>17215.4078947368</v>
       </c>
       <c r="AK214" s="0">
-        <v>11014.5175438596</v>
+        <v>1.10145175438597</v>
       </c>
       <c r="AL214" s="0">
         <v>2030.42352941176</v>
@@ -42317,7 +42317,7 @@
         <v>23285.1446540881</v>
       </c>
       <c r="AK215" s="0">
-        <v>11073.2722772277</v>
+        <v>1.10732722772277</v>
       </c>
       <c r="AL215" s="0">
         <v>9288.58682634731</v>
@@ -42512,7 +42512,7 @@
         <v>60596.5625</v>
       </c>
       <c r="AK216" s="0">
-        <v>42671.4285714286</v>
+        <v>4.26714285714286</v>
       </c>
       <c r="AL216" s="0">
         <v>2591.5625</v>
@@ -42707,7 +42707,7 @@
         <v>31264.7166666667</v>
       </c>
       <c r="AK217" s="0">
-        <v>21482.2063492064</v>
+        <v>2.14822063492064</v>
       </c>
       <c r="AL217" s="0">
         <v>2325.43609022556</v>
@@ -42902,7 +42902,7 @@
         <v>31995.1479289941</v>
       </c>
       <c r="AK218" s="0">
-        <v>15629.7803921569</v>
+        <v>1.56297803921569</v>
       </c>
       <c r="AL218" s="0">
         <v>4059.65714285714</v>
@@ -43097,7 +43097,7 @@
         <v>181242.848484848</v>
       </c>
       <c r="AK219" s="0">
-        <v>68625.4117647059</v>
+        <v>6.86254117647059</v>
       </c>
       <c r="AL219" s="0">
         <v>18119.875</v>
@@ -43292,7 +43292,7 @@
         <v>23408.0289855072</v>
       </c>
       <c r="AK220" s="0">
-        <v>9488.45833333333</v>
+        <v>0.948845833333333</v>
       </c>
       <c r="AL220" s="0">
         <v>11534.1333333333</v>
@@ -43487,7 +43487,7 @@
         <v>13054.5517241379</v>
       </c>
       <c r="AK221" s="0">
-        <v>7761.93333418997</v>
+        <v>0.776193333418997</v>
       </c>
       <c r="AL221" s="0">
         <v>3690.76923076923</v>
@@ -43682,7 +43682,7 @@
         <v>42211.1346153846</v>
       </c>
       <c r="AK222" s="0">
-        <v>27162.5458715596</v>
+        <v>2.71625458715596</v>
       </c>
       <c r="AL222" s="0">
         <v>8086.32926829268</v>
@@ -43877,7 +43877,7 @@
         <v>47075.7794383397</v>
       </c>
       <c r="AK223" s="0">
-        <v>28618.9089738895</v>
+        <v>2.86189089738895</v>
       </c>
       <c r="AL223" s="0">
         <v>4025.67796610169</v>
@@ -44072,7 +44072,7 @@
         <v>42452.7123287671</v>
       </c>
       <c r="AK224" s="0">
-        <v>23596.0163934426</v>
+        <v>2.35960163934426</v>
       </c>
       <c r="AL224" s="0">
         <v>1580</v>
@@ -44267,7 +44267,7 @@
         <v>33289.0505050505</v>
       </c>
       <c r="AK225" s="0">
-        <v>16226.9253731343</v>
+        <v>1.62269253731343</v>
       </c>
       <c r="AL225" s="0">
         <v>1521.10091743119</v>
@@ -44462,7 +44462,7 @@
         <v>35266.9072164948</v>
       </c>
       <c r="AK226" s="0">
-        <v>23192.6666666667</v>
+        <v>2.31926666666667</v>
       </c>
       <c r="AL226" s="0">
         <v>4052.63157894737</v>
@@ -44657,7 +44657,7 @@
         <v>28914.1425286655</v>
       </c>
       <c r="AK227" s="0">
-        <v>20205.0421874523</v>
+        <v>2.02050421874523</v>
       </c>
       <c r="AL227" s="0">
         <v>4129.69696969697</v>
@@ -44852,7 +44852,7 @@
         <v>72712.109375</v>
       </c>
       <c r="AK228" s="0">
-        <v>16898.670886076</v>
+        <v>1.6898670886076</v>
       </c>
       <c r="AL228" s="0">
         <v>50029.0625</v>
@@ -45047,7 +45047,7 @@
         <v>31873.7098975728</v>
       </c>
       <c r="AK229" s="0">
-        <v>21640.745349263</v>
+        <v>2.1640745349263</v>
       </c>
       <c r="AL229" s="0">
         <v>2364.89655172414</v>
@@ -45242,7 +45242,7 @@
         <v>17130.3376588983</v>
       </c>
       <c r="AK230" s="0">
-        <v>8373.01846078726</v>
+        <v>0.837301846078726</v>
       </c>
       <c r="AL230" s="0">
         <v>613.114754098361</v>
@@ -45437,7 +45437,7 @@
         <v>22821.9675675676</v>
       </c>
       <c r="AK231" s="0">
-        <v>13264.6416665536</v>
+        <v>1.32646416665536</v>
       </c>
       <c r="AL231" s="0">
         <v>6920.75757575758</v>
@@ -45632,7 +45632,7 @@
         <v>43058.623853211</v>
       </c>
       <c r="AK232" s="0">
-        <v>19790.2236842105</v>
+        <v>1.97902236842105</v>
       </c>
       <c r="AL232" s="0">
         <v>10689.9322033898</v>
@@ -45827,7 +45827,7 @@
         <v>36338.546875</v>
       </c>
       <c r="AK233" s="0">
-        <v>18124.6394421215</v>
+        <v>1.81246394421215</v>
       </c>
       <c r="AL233" s="0">
         <v>5504</v>
@@ -46022,7 +46022,7 @@
         <v>54568.9479166667</v>
       </c>
       <c r="AK234" s="0">
-        <v>29374</v>
+        <v>2.9374</v>
       </c>
       <c r="AL234" s="0">
         <v>8937.85087719298</v>
@@ -46217,7 +46217,7 @@
         <v>58377.4409826807</v>
       </c>
       <c r="AK235" s="0">
-        <v>33690.6537815382</v>
+        <v>3.36906537815382</v>
       </c>
       <c r="AL235" s="0">
         <v>6965.15217391304</v>
@@ -46412,7 +46412,7 @@
         <v>17388.3444444444</v>
       </c>
       <c r="AK236" s="0">
-        <v>9110.81746031746</v>
+        <v>0.911081746031746</v>
       </c>
       <c r="AL236" s="0">
         <v>3460.43956043956</v>
@@ -46607,7 +46607,7 @@
         <v>34487.3052793561</v>
       </c>
       <c r="AK237" s="0">
-        <v>17764.6586168411</v>
+        <v>1.77646586168411</v>
       </c>
       <c r="AL237" s="0">
         <v>8011.97350993377</v>
@@ -46802,7 +46802,7 @@
         <v>21379.6119402985</v>
       </c>
       <c r="AK238" s="0">
-        <v>16790.4444444444</v>
+        <v>1.67904444444444</v>
       </c>
       <c r="AL238" s="0">
         <v>2407.32394366197</v>
@@ -46997,7 +46997,7 @@
         <v>19995.8181818182</v>
       </c>
       <c r="AK239" s="0">
-        <v>15272.3461538462</v>
+        <v>1.52723461538462</v>
       </c>
       <c r="AL239" s="0">
         <v>2004.21052631579</v>
@@ -47192,7 +47192,7 @@
         <v>22299.5844155844</v>
       </c>
       <c r="AK240" s="0">
-        <v>15328.1553398058</v>
+        <v>1.53281553398058</v>
       </c>
       <c r="AL240" s="0">
         <v>5950.93975903615</v>
@@ -47387,7 +47387,7 @@
         <v>32136.953125</v>
       </c>
       <c r="AK241" s="0">
-        <v>20466.1051660517</v>
+        <v>2.04661051660517</v>
       </c>
       <c r="AL241" s="0">
         <v>2565.93922651934</v>
@@ -47582,7 +47582,7 @@
         <v>72707.6923076923</v>
       </c>
       <c r="AK242" s="0">
-        <v>37953.7631578947</v>
+        <v>3.79537631578947</v>
       </c>
       <c r="AL242" s="0">
         <v>18473.2142857143</v>
@@ -47777,7 +47777,7 @@
         <v>37134</v>
       </c>
       <c r="AK243" s="0">
-        <v>21468.7203389831</v>
+        <v>2.14687203389831</v>
       </c>
       <c r="AL243" s="0">
         <v>5855.59139784946</v>
@@ -47972,7 +47972,7 @@
         <v>22582.74609375</v>
       </c>
       <c r="AK244" s="0">
-        <v>11713.5251780192</v>
+        <v>1.17135251780192</v>
       </c>
       <c r="AL244" s="0">
         <v>1391.70149253731</v>
@@ -48167,7 +48167,7 @@
         <v>104279.191176471</v>
       </c>
       <c r="AK245" s="0">
-        <v>22172.1721311475</v>
+        <v>2.21721721311475</v>
       </c>
       <c r="AL245" s="0">
         <v>44326.0759493671</v>
@@ -48362,7 +48362,7 @@
         <v>33840.0425531915</v>
       </c>
       <c r="AK246" s="0">
-        <v>15640.8791946309</v>
+        <v>1.56408791946309</v>
       </c>
       <c r="AL246" s="0">
         <v>10642.8571428571</v>
@@ -48557,7 +48557,7 @@
         <v>14725.8815789474</v>
       </c>
       <c r="AK247" s="0">
-        <v>8941.4801980198</v>
+        <v>0.89414801980198</v>
       </c>
       <c r="AL247" s="0">
         <v>2035.0303030303</v>
@@ -48752,7 +48752,7 @@
         <v>39368.6961996064</v>
       </c>
       <c r="AK248" s="0">
-        <v>26442.0230001831</v>
+        <v>2.64420230001831</v>
       </c>
       <c r="AL248" s="0">
         <v>2813.6170212766</v>
@@ -48947,7 +48947,7 @@
         <v>34508.7536231884</v>
       </c>
       <c r="AK249" s="0">
-        <v>20278.415</v>
+        <v>2.0278415</v>
       </c>
       <c r="AL249" s="0">
         <v>4245.21472392638</v>
@@ -49142,7 +49142,7 @@
         <v>25335.1744186047</v>
       </c>
       <c r="AK250" s="0">
-        <v>16860.8384615385</v>
+        <v>1.68608384615385</v>
       </c>
       <c r="AL250" s="0">
         <v>3932.63157894737</v>
@@ -49337,7 +49337,7 @@
         <v>17991.5826771654</v>
       </c>
       <c r="AK251" s="0">
-        <v>10719.65625</v>
+        <v>1.071965625</v>
       </c>
       <c r="AL251" s="0">
         <v>1768.29927007299</v>
@@ -49532,7 +49532,7 @@
         <v>16436.091954023</v>
       </c>
       <c r="AK252" s="0">
-        <v>6431.52459016393</v>
+        <v>0.643152459016394</v>
       </c>
       <c r="AL252" s="0">
         <v>8171.20879120879</v>
@@ -49727,7 +49727,7 @@
         <v>25698.4042553192</v>
       </c>
       <c r="AK253" s="0">
-        <v>18531.328125</v>
+        <v>1.8531328125</v>
       </c>
       <c r="AL253" s="0">
         <v>3235.20408163265</v>
@@ -49922,7 +49922,7 @@
         <v>30977.5151515152</v>
       </c>
       <c r="AK254" s="0">
-        <v>15418.1025641026</v>
+        <v>1.54181025641026</v>
       </c>
       <c r="AL254" s="0">
         <v>7477.16417910448</v>
@@ -50117,7 +50117,7 @@
         <v>14850.985915493</v>
       </c>
       <c r="AK255" s="0">
-        <v>7047.03488372093</v>
+        <v>0.704703488372093</v>
       </c>
       <c r="AL255" s="0">
         <v>3631.90476190476</v>
@@ -50312,7 +50312,7 @@
         <v>35336.1967213115</v>
       </c>
       <c r="AK256" s="0">
-        <v>17643.1071428571</v>
+        <v>1.76431071428571</v>
       </c>
       <c r="AL256" s="0">
         <v>13545.5616438356</v>
@@ -50507,7 +50507,7 @@
         <v>7273.3</v>
       </c>
       <c r="AK257" s="0">
-        <v>3214.4962406015</v>
+        <v>0.32144962406015</v>
       </c>
       <c r="AL257" s="0">
         <v>2310.9243697479</v>
@@ -50702,7 +50702,7 @@
         <v>16005.1211042346</v>
       </c>
       <c r="AK258" s="0">
-        <v>7751.12725271148</v>
+        <v>0.775112725271148</v>
       </c>
       <c r="AL258" s="0">
         <v>3363.85537190083</v>
@@ -50897,7 +50897,7 @@
         <v>12281.1285714286</v>
       </c>
       <c r="AK259" s="0">
-        <v>9114.31067961165</v>
+        <v>0.911431067961165</v>
       </c>
       <c r="AL259" s="0">
         <v>1153.42391304348</v>
@@ -51092,7 +51092,7 @@
         <v>34946.3095238095</v>
       </c>
       <c r="AK260" s="0">
-        <v>16765.6209150327</v>
+        <v>1.67656209150327</v>
       </c>
       <c r="AL260" s="0">
         <v>1019.44444444444</v>
@@ -51287,7 +51287,7 @@
         <v>77431</v>
       </c>
       <c r="AK261" s="0">
-        <v>44045.9574468085</v>
+        <v>4.40459574468085</v>
       </c>
       <c r="AL261" s="0">
         <v>4254.54545454546</v>
@@ -51482,7 +51482,7 @@
         <v>40976.5625</v>
       </c>
       <c r="AK262" s="0">
-        <v>27637.8153846154</v>
+        <v>2.76378153846154</v>
       </c>
       <c r="AL262" s="0">
         <v>1041.50943396226</v>
@@ -51677,7 +51677,7 @@
         <v>33085.7897961675</v>
       </c>
       <c r="AK263" s="0">
-        <v>7463.04558832505</v>
+        <v>0.746304558832505</v>
       </c>
       <c r="AL263" s="0">
         <v>19204.8461538462</v>
@@ -51872,7 +51872,7 @@
         <v>63033.1034482759</v>
       </c>
       <c r="AK264" s="0">
-        <v>44896.7333333333</v>
+        <v>4.48967333333333</v>
       </c>
       <c r="AL264" s="0">
         <v>3139.28571428571</v>
@@ -52067,7 +52067,7 @@
         <v>43766.2857142857</v>
       </c>
       <c r="AK265" s="0">
-        <v>24655.4</v>
+        <v>2.46554</v>
       </c>
       <c r="AL265" s="0">
         <v>7548.51063829787</v>
@@ -52262,7 +52262,7 @@
         <v>16948.0754716981</v>
       </c>
       <c r="AK266" s="0">
-        <v>7493.12941176471</v>
+        <v>0.749312941176471</v>
       </c>
       <c r="AL266" s="0">
         <v>4912.53333333333</v>
@@ -52457,7 +52457,7 @@
         <v>20677.5</v>
       </c>
       <c r="AK267" s="0">
-        <v>6110.32710280374</v>
+        <v>0.611032710280374</v>
       </c>
       <c r="AL267" s="0">
         <v>7938.33333333333</v>
@@ -52652,7 +52652,7 @@
         <v>32112.6976744186</v>
       </c>
       <c r="AK268" s="0">
-        <v>15856.7402597403</v>
+        <v>1.58567402597403</v>
       </c>
       <c r="AL268" s="0">
         <v>3566.66666666667</v>
@@ -52847,7 +52847,7 @@
         <v>21531.6455269608</v>
       </c>
       <c r="AK269" s="0">
-        <v>11138.3895996094</v>
+        <v>1.11383895996094</v>
       </c>
       <c r="AL269" s="0">
         <v>5889.39759036145</v>
@@ -53042,7 +53042,7 @@
         <v>28344.7547169811</v>
       </c>
       <c r="AK270" s="0">
-        <v>15708.0421781994</v>
+        <v>1.57080421781994</v>
       </c>
       <c r="AL270" s="0">
         <v>2650.35714285714</v>
@@ -53237,7 +53237,7 @@
         <v>17401.3722195095</v>
       </c>
       <c r="AK271" s="0">
-        <v>14255.9023257707</v>
+        <v>1.42559023257707</v>
       </c>
       <c r="AL271" s="0">
         <v>910.434782608696</v>
@@ -53432,7 +53432,7 @@
         <v>28268.6153846154</v>
       </c>
       <c r="AK272" s="0">
-        <v>13676.2818181818</v>
+        <v>1.36762818181818</v>
       </c>
       <c r="AL272" s="0">
         <v>4432.67326732673</v>
@@ -53627,7 +53627,7 @@
         <v>12374.4671532847</v>
       </c>
       <c r="AK273" s="0">
-        <v>3537.88617886179</v>
+        <v>0.353788617886179</v>
       </c>
       <c r="AL273" s="0">
         <v>6151.07317073171</v>
@@ -53822,7 +53822,7 @@
         <v>14179.3939393939</v>
       </c>
       <c r="AK274" s="0">
-        <v>11134.8387096774</v>
+        <v>1.11348387096774</v>
       </c>
       <c r="AL274" s="0">
         <v>5389.83050847458</v>
@@ -54017,7 +54017,7 @@
         <v>16025.7619047619</v>
       </c>
       <c r="AK275" s="0">
-        <v>7474.37931034483</v>
+        <v>0.747437931034483</v>
       </c>
       <c r="AL275" s="0">
         <v>4010.01869158879</v>
@@ -54212,7 +54212,7 @@
         <v>14668.2</v>
       </c>
       <c r="AK276" s="0">
-        <v>4717.47572815534</v>
+        <v>0.471747572815534</v>
       </c>
       <c r="AL276" s="0">
         <v>9412.94117647059</v>
@@ -54407,7 +54407,7 @@
         <v>12926.2542372881</v>
       </c>
       <c r="AK277" s="0">
-        <v>9235.18</v>
+        <v>0.923518</v>
       </c>
       <c r="AL277" s="0">
         <v>1705.44444444444</v>
@@ -54602,7 +54602,7 @@
         <v>75955.3333333333</v>
       </c>
       <c r="AK278" s="0">
-        <v>34170.0119047619</v>
+        <v>3.41700119047619</v>
       </c>
       <c r="AL278" s="0">
         <v>8474.92753623188</v>
@@ -54797,7 +54797,7 @@
         <v>21481.306122449</v>
       </c>
       <c r="AK279" s="0">
-        <v>12023.1894736842</v>
+        <v>1.20231894736842</v>
       </c>
       <c r="AL279" s="0">
         <v>96.5853658536585</v>
@@ -54992,7 +54992,7 @@
         <v>15750.0256410256</v>
       </c>
       <c r="AK280" s="0">
-        <v>6926.14912280702</v>
+        <v>0.692614912280702</v>
       </c>
       <c r="AL280" s="0">
         <v>2021.20720720721</v>
@@ -55187,7 +55187,7 @@
         <v>11983.2292659108</v>
       </c>
       <c r="AK281" s="0">
-        <v>3952.78148142497</v>
+        <v>0.395278148142497</v>
       </c>
       <c r="AL281" s="0">
         <v>3569.25925925926</v>
@@ -55382,7 +55382,7 @@
         <v>15102.1866666667</v>
       </c>
       <c r="AK282" s="0">
-        <v>9585.59842519685</v>
+        <v>0.958559842519685</v>
       </c>
       <c r="AL282" s="0">
         <v>1732.43564356436</v>
@@ -55577,7 +55577,7 @@
         <v>11292.7346938776</v>
       </c>
       <c r="AK283" s="0">
-        <v>5081.03035736084</v>
+        <v>0.508103035736084</v>
       </c>
       <c r="AL283" s="0">
         <v>1164</v>
@@ -55772,7 +55772,7 @@
         <v>37565.5</v>
       </c>
       <c r="AK284" s="0">
-        <v>20980.3891518803</v>
+        <v>2.09803891518803</v>
       </c>
       <c r="AL284" s="0">
         <v>2619.04761904762</v>
@@ -55967,7 +55967,7 @@
         <v>58449.0909090909</v>
       </c>
       <c r="AK285" s="0">
-        <v>30250.9787234043</v>
+        <v>3.02509787234043</v>
       </c>
       <c r="AL285" s="0">
         <v>8027.90697674419</v>
@@ -56162,7 +56162,7 @@
         <v>51658.1818181818</v>
       </c>
       <c r="AK286" s="0">
-        <v>22795.3058938419</v>
+        <v>2.27953058938419</v>
       </c>
       <c r="AL286" s="0">
         <v>0</v>
@@ -56357,7 +56357,7 @@
         <v>46919.5</v>
       </c>
       <c r="AK287" s="0">
-        <v>24648.3529411765</v>
+        <v>2.46483529411765</v>
       </c>
       <c r="AL287" s="0">
         <v>4588.23529411765</v>
@@ -56552,7 +56552,7 @@
         <v>14562.60930119</v>
       </c>
       <c r="AK288" s="0">
-        <v>7783.37185149016</v>
+        <v>0.778337185149016</v>
       </c>
       <c r="AL288" s="0">
         <v>3994.18803418803</v>
@@ -56747,7 +56747,7 @@
         <v>20447.5744680851</v>
       </c>
       <c r="AK289" s="0">
-        <v>7689.30303030303</v>
+        <v>0.768930303030303</v>
       </c>
       <c r="AL289" s="0">
         <v>2957.38636363636</v>
@@ -56942,7 +56942,7 @@
         <v>106422.476190476</v>
       </c>
       <c r="AK290" s="0">
-        <v>65891.1794871795</v>
+        <v>6.58911794871795</v>
       </c>
       <c r="AL290" s="0">
         <v>0</v>
@@ -57137,7 +57137,7 @@
         <v>8502.55263157895</v>
       </c>
       <c r="AK291" s="0">
-        <v>3376.33</v>
+        <v>0.337633</v>
       </c>
       <c r="AL291" s="0">
         <v>1684.18987341772</v>
@@ -57332,7 +57332,7 @@
         <v>97743.75</v>
       </c>
       <c r="AK292" s="0">
-        <v>37722.5</v>
+        <v>3.77225</v>
       </c>
       <c r="AL292" s="0">
         <v>8828.10810810811</v>
@@ -57527,7 +57527,7 @@
         <v>24924.0602409639</v>
       </c>
       <c r="AK293" s="0">
-        <v>13245.9857651246</v>
+        <v>1.32459857651246</v>
       </c>
       <c r="AL293" s="0">
         <v>3984.34024896266</v>
@@ -57722,7 +57722,7 @@
         <v>65077.9428571429</v>
       </c>
       <c r="AK294" s="0">
-        <v>48464.1785714286</v>
+        <v>4.84641785714286</v>
       </c>
       <c r="AL294" s="0">
         <v>11854.9019607843</v>
@@ -57917,7 +57917,7 @@
         <v>19996.4847483915</v>
       </c>
       <c r="AK295" s="0">
-        <v>11381.9430938406</v>
+        <v>1.13819430938406</v>
       </c>
       <c r="AL295" s="0">
         <v>3238.9247311828</v>
@@ -58112,7 +58112,7 @@
         <v>23138.1851851852</v>
       </c>
       <c r="AK296" s="0">
-        <v>11687.1092436975</v>
+        <v>1.16871092436975</v>
       </c>
       <c r="AL296" s="0">
         <v>1228.07692307692</v>
@@ -58307,7 +58307,7 @@
         <v>12697.3599877451</v>
       </c>
       <c r="AK297" s="0">
-        <v>5001.3123337766</v>
+        <v>0.50013123337766</v>
       </c>
       <c r="AL297" s="0">
         <v>4604.7619047619</v>
@@ -58502,7 +58502,7 @@
         <v>45014.7826086957</v>
       </c>
       <c r="AK298" s="0">
-        <v>19857.3333333333</v>
+        <v>1.98573333333333</v>
       </c>
       <c r="AL298" s="0">
         <v>5863.63636363636</v>
@@ -58697,7 +58697,7 @@
         <v>49745.1342037671</v>
       </c>
       <c r="AK299" s="0">
-        <v>24628.0649124949</v>
+        <v>2.46280649124949</v>
       </c>
       <c r="AL299" s="0">
         <v>8589.70297029703</v>
@@ -58892,7 +58892,7 @@
         <v>35665.5616592751</v>
       </c>
       <c r="AK300" s="0">
-        <v>16161.3298674727</v>
+        <v>1.61613298674727</v>
       </c>
       <c r="AL300" s="0">
         <v>10459.7</v>
@@ -59087,7 +59087,7 @@
         <v>43634.6666666667</v>
       </c>
       <c r="AK301" s="0">
-        <v>33671.0588235294</v>
+        <v>3.36710588235294</v>
       </c>
       <c r="AL301" s="0">
         <v>11844.6153846154</v>
@@ -59282,7 +59282,7 @@
         <v>46210.0952380952</v>
       </c>
       <c r="AK302" s="0">
-        <v>24221.0285714286</v>
+        <v>2.42210285714286</v>
       </c>
       <c r="AL302" s="0">
         <v>16929.0322580645</v>
@@ -59477,7 +59477,7 @@
         <v>40627.3724407328</v>
       </c>
       <c r="AK303" s="0">
-        <v>24623.0058451186</v>
+        <v>2.46230058451186</v>
       </c>
       <c r="AL303" s="0">
         <v>1383.61538461538</v>
@@ -59672,7 +59672,7 @@
         <v>19623.8461538462</v>
       </c>
       <c r="AK304" s="0">
-        <v>10781.1722628183</v>
+        <v>1.07811722628183</v>
       </c>
       <c r="AL304" s="0">
         <v>2102.66129032258</v>
@@ -59867,7 +59867,7 @@
         <v>22545.9220779221</v>
       </c>
       <c r="AK305" s="0">
-        <v>10892.7614678899</v>
+        <v>1.08927614678899</v>
       </c>
       <c r="AL305" s="0">
         <v>4258.64646464646</v>
@@ -60062,7 +60062,7 @@
         <v>43426.5161290323</v>
       </c>
       <c r="AK306" s="0">
-        <v>17417.6527777778</v>
+        <v>1.74176527777778</v>
       </c>
       <c r="AL306" s="0">
         <v>1377.35294117647</v>
@@ -60257,7 +60257,7 @@
         <v>24386.4864864865</v>
       </c>
       <c r="AK307" s="0">
-        <v>15950.625</v>
+        <v>1.5950625</v>
       </c>
       <c r="AL307" s="0">
         <v>1366.77966101695</v>
@@ -60452,7 +60452,7 @@
         <v>29529.5208333333</v>
       </c>
       <c r="AK308" s="0">
-        <v>12532.3010752688</v>
+        <v>1.25323010752688</v>
       </c>
       <c r="AL308" s="0">
         <v>11583.4210526316</v>
@@ -60647,7 +60647,7 @@
         <v>22698.2330097087</v>
       </c>
       <c r="AK309" s="0">
-        <v>11625.0243902439</v>
+        <v>1.16250243902439</v>
       </c>
       <c r="AL309" s="0">
         <v>5826.14864864865</v>
@@ -60842,7 +60842,7 @@
         <v>64629.0909090909</v>
       </c>
       <c r="AK310" s="0">
-        <v>34289.5384615385</v>
+        <v>3.42895384615385</v>
       </c>
       <c r="AL310" s="0">
         <v>3750</v>
@@ -61037,7 +61037,7 @@
         <v>8144.93077674279</v>
       </c>
       <c r="AK311" s="0">
-        <v>3626.8413787491</v>
+        <v>0.36268413787491</v>
       </c>
       <c r="AL311" s="0">
         <v>3617.27777777778</v>
@@ -61232,7 +61232,7 @@
         <v>24180.1403508772</v>
       </c>
       <c r="AK312" s="0">
-        <v>14300.8086956522</v>
+        <v>1.43008086956522</v>
       </c>
       <c r="AL312" s="0">
         <v>3058.82352941176</v>
@@ -61427,7 +61427,7 @@
         <v>14180.2028985507</v>
       </c>
       <c r="AK313" s="0">
-        <v>5438.71171171171</v>
+        <v>0.543871171171171</v>
       </c>
       <c r="AL313" s="0">
         <v>2082.1359223301</v>
@@ -61622,7 +61622,7 @@
         <v>41103.7</v>
       </c>
       <c r="AK314" s="0">
-        <v>8459.71621621622</v>
+        <v>0.845971621621622</v>
       </c>
       <c r="AL314" s="0">
         <v>9190.78947368421</v>
@@ -61817,7 +61817,7 @@
         <v>13600.6510067114</v>
       </c>
       <c r="AK315" s="0">
-        <v>7451.15909090909</v>
+        <v>0.745115909090909</v>
       </c>
       <c r="AL315" s="0">
         <v>2175.79881656805</v>
@@ -62012,7 +62012,7 @@
         <v>21587.2765957447</v>
       </c>
       <c r="AK316" s="0">
-        <v>6993.02272727273</v>
+        <v>0.699302272727273</v>
       </c>
       <c r="AL316" s="0">
         <v>6678.08823529412</v>
@@ -62207,7 +62207,7 @@
         <v>25311.5714285714</v>
       </c>
       <c r="AK317" s="0">
-        <v>9416.21052631579</v>
+        <v>0.941621052631579</v>
       </c>
       <c r="AL317" s="0">
         <v>7115.04132231405</v>
@@ -62402,7 +62402,7 @@
         <v>17612.431168197</v>
       </c>
       <c r="AK318" s="0">
-        <v>9282.84999992434</v>
+        <v>0.928284999992434</v>
       </c>
       <c r="AL318" s="0">
         <v>3720.40952380952</v>
@@ -62597,7 +62597,7 @@
         <v>19714.484375</v>
       </c>
       <c r="AK319" s="0">
-        <v>7883.47096761068</v>
+        <v>0.788347096761068</v>
       </c>
       <c r="AL319" s="0">
         <v>5210.9</v>
@@ -62792,7 +62792,7 @@
         <v>28416.3333333333</v>
       </c>
       <c r="AK320" s="0">
-        <v>8370.19417475728</v>
+        <v>0.837019417475728</v>
       </c>
       <c r="AL320" s="0">
         <v>4626.15189873418</v>
@@ -62987,7 +62987,7 @@
         <v>35587.7014925373</v>
       </c>
       <c r="AK321" s="0">
-        <v>16433.1006711409</v>
+        <v>1.64331006711409</v>
       </c>
       <c r="AL321" s="0">
         <v>6044.87218045113</v>
@@ -63182,7 +63182,7 @@
         <v>24493.6315789474</v>
       </c>
       <c r="AK322" s="0">
-        <v>13442.1495726496</v>
+        <v>1.34421495726496</v>
       </c>
       <c r="AL322" s="0">
         <v>2057.36994219653</v>
@@ -63377,7 +63377,7 @@
         <v>14238.7666666667</v>
       </c>
       <c r="AK323" s="0">
-        <v>5831.95833333333</v>
+        <v>0.583195833333333</v>
       </c>
       <c r="AL323" s="0">
         <v>1510.18604651163</v>
@@ -63572,7 +63572,7 @@
         <v>31975.581108941</v>
       </c>
       <c r="AK324" s="0">
-        <v>16111.8165377103</v>
+        <v>1.61118165377103</v>
       </c>
       <c r="AL324" s="0">
         <v>8741.86597938144</v>
@@ -63767,7 +63767,7 @@
         <v>40968.7733333333</v>
       </c>
       <c r="AK325" s="0">
-        <v>18055.950617284</v>
+        <v>1.8055950617284</v>
       </c>
       <c r="AL325" s="0">
         <v>4361.79104477612</v>
@@ -63962,7 +63962,7 @@
         <v>11473.0856542223</v>
       </c>
       <c r="AK326" s="0">
-        <v>4804.92388412327</v>
+        <v>0.480492388412327</v>
       </c>
       <c r="AL326" s="0">
         <v>2295.79591836735</v>
@@ -64157,7 +64157,7 @@
         <v>46883.4666666667</v>
       </c>
       <c r="AK327" s="0">
-        <v>19425.6923076923</v>
+        <v>1.94256923076923</v>
       </c>
       <c r="AL327" s="0">
         <v>9007.62962962963</v>
@@ -64352,7 +64352,7 @@
         <v>4920.55714285714</v>
       </c>
       <c r="AK328" s="0">
-        <v>3247.895651997</v>
+        <v>0.3247895651997</v>
       </c>
       <c r="AL328" s="0">
         <v>401.018181818182</v>
@@ -64547,7 +64547,7 @@
         <v>97286.6956521739</v>
       </c>
       <c r="AK329" s="0">
-        <v>53672.8245614035</v>
+        <v>5.36728245614035</v>
       </c>
       <c r="AL329" s="0">
         <v>12417.4757281553</v>
@@ -64742,7 +64742,7 @@
         <v>25679.4642857143</v>
       </c>
       <c r="AK330" s="0">
-        <v>14056.1607142857</v>
+        <v>1.40561607142857</v>
       </c>
       <c r="AL330" s="0">
         <v>2406.73469387755</v>
@@ -64937,7 +64937,7 @@
         <v>10879.8961038961</v>
       </c>
       <c r="AK331" s="0">
-        <v>4862.76716408801</v>
+        <v>0.486276716408801</v>
       </c>
       <c r="AL331" s="0">
         <v>2655.68965517241</v>
@@ -65132,7 +65132,7 @@
         <v>10038.7878787879</v>
       </c>
       <c r="AK332" s="0">
-        <v>4756.14761904762</v>
+        <v>0.475614761904762</v>
       </c>
       <c r="AL332" s="0">
         <v>1295.21276595745</v>
@@ -65327,7 +65327,7 @@
         <v>124359.682539683</v>
       </c>
       <c r="AK333" s="0">
-        <v>15276.1367521368</v>
+        <v>1.52761367521368</v>
       </c>
       <c r="AL333" s="0">
         <v>67101.1224489796</v>
@@ -65522,7 +65522,7 @@
         <v>21786.4516129032</v>
       </c>
       <c r="AK334" s="0">
-        <v>7605.98214285714</v>
+        <v>0.760598214285714</v>
       </c>
       <c r="AL334" s="0">
         <v>5084.89795918367</v>
@@ -65717,7 +65717,7 @@
         <v>16016.8965517241</v>
       </c>
       <c r="AK335" s="0">
-        <v>8752.83561643836</v>
+        <v>0.875283561643836</v>
       </c>
       <c r="AL335" s="0">
         <v>3446.15873015873</v>
@@ -65912,7 +65912,7 @@
         <v>8022.61363636364</v>
       </c>
       <c r="AK336" s="0">
-        <v>3930.18390804598</v>
+        <v>0.393018390804598</v>
       </c>
       <c r="AL336" s="0">
         <v>4361.51315789474</v>
@@ -66107,7 +66107,7 @@
         <v>73682.7407407407</v>
       </c>
       <c r="AK337" s="0">
-        <v>31639.2244897959</v>
+        <v>3.16392244897959</v>
       </c>
       <c r="AL337" s="0">
         <v>5800</v>
@@ -66302,7 +66302,7 @@
         <v>16081.3043478261</v>
       </c>
       <c r="AK338" s="0">
-        <v>11338.2524594166</v>
+        <v>1.13382524594166</v>
       </c>
       <c r="AL338" s="0">
         <v>3593.86666666667</v>
@@ -66497,7 +66497,7 @@
         <v>90759.5</v>
       </c>
       <c r="AK339" s="0">
-        <v>43116.9756097561</v>
+        <v>4.31169756097561</v>
       </c>
       <c r="AL339" s="0">
         <v>9690.32258064516</v>
@@ -66692,7 +66692,7 @@
         <v>16719.6333333333</v>
       </c>
       <c r="AK340" s="0">
-        <v>8164.40833333333</v>
+        <v>0.816440833333333</v>
       </c>
       <c r="AL340" s="0">
         <v>3549.12844036697</v>
@@ -66887,7 +66887,7 @@
         <v>12742.437037037</v>
       </c>
       <c r="AK341" s="0">
-        <v>7123.73658536585</v>
+        <v>0.712373658536585</v>
       </c>
       <c r="AL341" s="0">
         <v>2777.02105263158</v>
@@ -67082,7 +67082,7 @@
         <v>76650</v>
       </c>
       <c r="AK342" s="0">
-        <v>30754.6666666667</v>
+        <v>3.07546666666667</v>
       </c>
       <c r="AL342" s="0">
         <v>0</v>
@@ -67277,7 +67277,7 @@
         <v>21519.4260869565</v>
       </c>
       <c r="AK343" s="0">
-        <v>12962.1450777202</v>
+        <v>1.29621450777202</v>
       </c>
       <c r="AL343" s="0">
         <v>1717.06896551724</v>
@@ -67472,7 +67472,7 @@
         <v>20991.0843373494</v>
       </c>
       <c r="AK344" s="0">
-        <v>9230.84188034188</v>
+        <v>0.923084188034188</v>
       </c>
       <c r="AL344" s="0">
         <v>5228.71748878924</v>
@@ -67667,7 +67667,7 @@
         <v>94127.32796875</v>
       </c>
       <c r="AK345" s="0">
-        <v>35683.6216980556</v>
+        <v>3.56836216980556</v>
       </c>
       <c r="AL345" s="0">
         <v>22457.92</v>
@@ -67862,7 +67862,7 @@
         <v>12052.4937496185</v>
       </c>
       <c r="AK346" s="0">
-        <v>7309.02745026233</v>
+        <v>0.730902745026233</v>
       </c>
       <c r="AL346" s="0">
         <v>1084.40860215054</v>
@@ -68057,7 +68057,7 @@
         <v>6165.07407407407</v>
       </c>
       <c r="AK347" s="0">
-        <v>3297.43157894737</v>
+        <v>0.329743157894737</v>
       </c>
       <c r="AL347" s="0">
         <v>1660.40476190476</v>
@@ -68252,7 +68252,7 @@
         <v>39221.993006993</v>
       </c>
       <c r="AK348" s="0">
-        <v>22070.9777777778</v>
+        <v>2.20709777777778</v>
       </c>
       <c r="AL348" s="0">
         <v>5877.10714285714</v>
@@ -68447,7 +68447,7 @@
         <v>51436.8951646959</v>
       </c>
       <c r="AK349" s="0">
-        <v>24091.7281110003</v>
+        <v>2.40917281110003</v>
       </c>
       <c r="AL349" s="0">
         <v>4181.62962962963</v>
@@ -68642,7 +68642,7 @@
         <v>41260.4761904762</v>
       </c>
       <c r="AK350" s="0">
-        <v>18422.8910891089</v>
+        <v>1.84228910891089</v>
       </c>
       <c r="AL350" s="0">
         <v>2756.97802197802</v>
@@ -68837,7 +68837,7 @@
         <v>38964.9350649351</v>
       </c>
       <c r="AK351" s="0">
-        <v>20606.6938712828</v>
+        <v>2.06066938712828</v>
       </c>
       <c r="AL351" s="0">
         <v>4384.77876106195</v>
@@ -69032,7 +69032,7 @@
         <v>43737.5061848958</v>
       </c>
       <c r="AK352" s="0">
-        <v>16052.6429632482</v>
+        <v>1.60526429632482</v>
       </c>
       <c r="AL352" s="0">
         <v>10137.7099236641</v>
@@ -69227,7 +69227,7 @@
         <v>18059.9104477612</v>
       </c>
       <c r="AK353" s="0">
-        <v>7828.9173553719</v>
+        <v>0.78289173553719</v>
       </c>
       <c r="AL353" s="0">
         <v>2670.38095238095</v>
@@ -69422,7 +69422,7 @@
         <v>24741.4</v>
       </c>
       <c r="AK354" s="0">
-        <v>9329.54545454545</v>
+        <v>0.932954545454545</v>
       </c>
       <c r="AL354" s="0">
         <v>21422.8070175439</v>
@@ -69617,7 +69617,7 @@
         <v>18298.9288845486</v>
       </c>
       <c r="AK355" s="0">
-        <v>16753.7345915021</v>
+        <v>1.67537345915021</v>
       </c>
       <c r="AL355" s="0">
         <v>2142.68115942029</v>
@@ -69812,7 +69812,7 @@
         <v>15062.2392861503</v>
       </c>
       <c r="AK356" s="0">
-        <v>8225.36423081618</v>
+        <v>0.822536423081618</v>
       </c>
       <c r="AL356" s="0">
         <v>592.715789473684</v>
@@ -70007,7 +70007,7 @@
         <v>6466.19266055046</v>
       </c>
       <c r="AK357" s="0">
-        <v>2564.21081081081</v>
+        <v>0.256421081081081</v>
       </c>
       <c r="AL357" s="0">
         <v>3574.09638554217</v>
@@ -70202,7 +70202,7 @@
         <v>35601.7978830645</v>
       </c>
       <c r="AK358" s="0">
-        <v>18522.8276893029</v>
+        <v>1.85228276893029</v>
       </c>
       <c r="AL358" s="0">
         <v>5439.49206349206</v>
@@ -70397,7 +70397,7 @@
         <v>41151.8787878788</v>
       </c>
       <c r="AK359" s="0">
-        <v>19488.8648648649</v>
+        <v>1.94888648648649</v>
       </c>
       <c r="AL359" s="0">
         <v>2806.25</v>
@@ -70592,7 +70592,7 @@
         <v>38132.7543945313</v>
       </c>
       <c r="AK360" s="0">
-        <v>25728.1947423031</v>
+        <v>2.57281947423031</v>
       </c>
       <c r="AL360" s="0">
         <v>8789.36363636364</v>
@@ -70787,7 +70787,7 @@
         <v>45113.2753623188</v>
       </c>
       <c r="AK361" s="0">
-        <v>24027.487804878</v>
+        <v>2.4027487804878</v>
       </c>
       <c r="AL361" s="0">
         <v>4412.64957264957</v>
@@ -70982,7 +70982,7 @@
         <v>12283.4696969697</v>
       </c>
       <c r="AK362" s="0">
-        <v>5737.80508474576</v>
+        <v>0.573780508474576</v>
       </c>
       <c r="AL362" s="0">
         <v>726.126126126126</v>
@@ -71177,7 +71177,7 @@
         <v>19957.7159441519</v>
       </c>
       <c r="AK363" s="0">
-        <v>9399.37969529205</v>
+        <v>0.939937969529205</v>
       </c>
       <c r="AL363" s="0">
         <v>3913.40909090909</v>
@@ -71372,7 +71372,7 @@
         <v>8255.41463414634</v>
       </c>
       <c r="AK364" s="0">
-        <v>5365.13043478261</v>
+        <v>0.536513043478261</v>
       </c>
       <c r="AL364" s="0">
         <v>408.148648648649</v>
@@ -71567,7 +71567,7 @@
         <v>16035.4126984127</v>
       </c>
       <c r="AK365" s="0">
-        <v>8310.97058823529</v>
+        <v>0.831097058823529</v>
       </c>
       <c r="AL365" s="0">
         <v>6013.39784946237</v>
@@ -71762,7 +71762,7 @@
         <v>4971.36363636364</v>
       </c>
       <c r="AK366" s="0">
-        <v>6480</v>
+        <v>0.648</v>
       </c>
       <c r="AL366" s="0">
         <v>-2751.48936170213</v>
@@ -71957,7 +71957,7 @@
         <v>24822.6923076923</v>
       </c>
       <c r="AK367" s="0">
-        <v>11757.4196078431</v>
+        <v>1.17574196078431</v>
       </c>
       <c r="AL367" s="0">
         <v>3472.80213903743</v>
@@ -72152,7 +72152,7 @@
         <v>86828.6666666667</v>
       </c>
       <c r="AK368" s="0">
-        <v>51031.012987013</v>
+        <v>5.1031012987013</v>
       </c>
       <c r="AL368" s="0">
         <v>10300</v>
@@ -72347,7 +72347,7 @@
         <v>30394.5479452055</v>
       </c>
       <c r="AK369" s="0">
-        <v>12673.1696428571</v>
+        <v>1.26731696428571</v>
       </c>
       <c r="AL369" s="0">
         <v>4909.49056603774</v>
@@ -72542,7 +72542,7 @@
         <v>17791.3913043478</v>
       </c>
       <c r="AK370" s="0">
-        <v>7886.96046518725</v>
+        <v>0.788696046518725</v>
       </c>
       <c r="AL370" s="0">
         <v>2116.1875</v>
@@ -72737,7 +72737,7 @@
         <v>18417.7419354839</v>
       </c>
       <c r="AK371" s="0">
-        <v>98847.4576271186</v>
+        <v>9.88474576271186</v>
       </c>
       <c r="AL371" s="0">
         <v>-9670.59405940594</v>
@@ -72932,7 +72932,7 @@
         <v>22725.039612409</v>
       </c>
       <c r="AK372" s="0">
-        <v>9880.85544812433</v>
+        <v>0.988085544812433</v>
       </c>
       <c r="AL372" s="0">
         <v>3454.14814814815</v>
@@ -73127,7 +73127,7 @@
         <v>9732.2</v>
       </c>
       <c r="AK373" s="0">
-        <v>4990.12807881773</v>
+        <v>0.499012807881773</v>
       </c>
       <c r="AL373" s="0">
         <v>2111.42045454545</v>
@@ -73322,7 +73322,7 @@
         <v>34276.6842105263</v>
       </c>
       <c r="AK374" s="0">
-        <v>23841.4734042553</v>
+        <v>2.38414734042553</v>
       </c>
       <c r="AL374" s="0">
         <v>3179.60248447205</v>
@@ -73517,7 +73517,7 @@
         <v>23377.1885245902</v>
       </c>
       <c r="AK375" s="0">
-        <v>10395.546728972</v>
+        <v>1.0395546728972</v>
       </c>
       <c r="AL375" s="0">
         <v>5471.60621761658</v>
@@ -73712,7 +73712,7 @@
         <v>15287.9411764706</v>
       </c>
       <c r="AK376" s="0">
-        <v>7591.34126984127</v>
+        <v>0.759134126984127</v>
       </c>
       <c r="AL376" s="0">
         <v>4284.34782608696</v>
@@ -73907,7 +73907,7 @@
         <v>11220.5784585806</v>
       </c>
       <c r="AK377" s="0">
-        <v>5966.98026944513</v>
+        <v>0.596698026944513</v>
       </c>
       <c r="AL377" s="0">
         <v>2164.54545454545</v>
@@ -74102,7 +74102,7 @@
         <v>8440.38095238095</v>
       </c>
       <c r="AK378" s="0">
-        <v>4596.28666687012</v>
+        <v>0.459628666687012</v>
       </c>
       <c r="AL378" s="0">
         <v>2651.35135135135</v>
@@ -74297,7 +74297,7 @@
         <v>21004.5974025974</v>
       </c>
       <c r="AK379" s="0">
-        <v>10613.4263565891</v>
+        <v>1.06134263565891</v>
       </c>
       <c r="AL379" s="0">
         <v>8744.58333333333</v>

</xml_diff>